<commit_message>
Sales Forecast Update, for all three product divisions
</commit_message>
<xml_diff>
--- a/database/Beezniss_Forecast_2018.xlsx
+++ b/database/Beezniss_Forecast_2018.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thor-from-Asgard\Desktop\beezniss\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D48D589E-8A28-4F42-980B-0ED11BE9A792}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FcstMonthlyFY2018" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <sheet name="FcstQtrMitochonFY2018" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_Sheet1A6N91" hidden="1">FcstMonthlyFY2018!$A$4:$N$7</definedName>
+    <definedName name="_xlcn.WorksheetConnection_Sheet1A6N9" hidden="1">FcstMonthlyFY2018!$A$4:$N$7</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,8 +39,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="ThisWorkbookDataModel" description="Data Model" type="5" refreshedVersion="6" minRefreshableVersion="5" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="ThisWorkbookDataModel" description="Data Model" type="5" refreshedVersion="6" minRefreshableVersion="5" background="1">
     <dbPr connection="Data Model Connection" command="Model" commandType="1"/>
     <olapPr sendLocale="1" rowDrillCount="1000"/>
     <extLst>
@@ -48,11 +49,11 @@
       </ext>
     </extLst>
   </connection>
-  <connection id="2" name="WorksheetConnection_Sheet1!$A$6:$N$9" type="102" refreshedVersion="6" minRefreshableVersion="5">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="WorksheetConnection_Sheet1!$A$6:$N$9" type="102" refreshedVersion="6" minRefreshableVersion="5">
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Sheet1A6N91"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Sheet1A6N9"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="31">
   <si>
     <t>Chocolate Chip Cookies</t>
   </si>
@@ -154,13 +155,13 @@
     <t>5</t>
   </si>
   <si>
-    <t>2018-03-30</t>
+    <t>2018-04-26</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -458,37 +459,37 @@
                   <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1060</c:v>
+                  <c:v>1040</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1123.6000000000001</c:v>
+                  <c:v>1081.6000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1191.0160000000003</c:v>
+                  <c:v>1124.8640000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1262.4769600000004</c:v>
+                  <c:v>1169.8585600000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1338.2255776000004</c:v>
+                  <c:v>1216.6529024000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1418.5191122560004</c:v>
+                  <c:v>1265.3190184960004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1503.6302589913605</c:v>
+                  <c:v>1315.9317792358404</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1593.8480745308423</c:v>
+                  <c:v>1368.5690504052741</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1689.4789590026928</c:v>
+                  <c:v>1423.311812421485</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1790.8476965428545</c:v>
+                  <c:v>1480.2442849183444</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1898.2985583354259</c:v>
+                  <c:v>1539.4540563150783</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -578,37 +579,37 @@
                   <c:v>1100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1166</c:v>
+                  <c:v>1144</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1235.96</c:v>
+                  <c:v>1189.76</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1310.1176</c:v>
+                  <c:v>1237.3504</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1388.7246560000001</c:v>
+                  <c:v>1286.8444160000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1472.0481353600003</c:v>
+                  <c:v>1338.3181926400002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1560.3710234816003</c:v>
+                  <c:v>1391.8509203456003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1653.9932848904964</c:v>
+                  <c:v>1447.5249571594245</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1753.2328819839263</c:v>
+                  <c:v>1505.4259554458015</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1858.4268549029618</c:v>
+                  <c:v>1565.6429936636337</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1969.9324661971395</c:v>
+                  <c:v>1628.2687134101791</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2088.128414168968</c:v>
+                  <c:v>1693.3994619465864</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -698,37 +699,37 @@
                   <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>742</c:v>
+                  <c:v>728</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>786.5200000000001</c:v>
+                  <c:v>757.12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>833.71120000000019</c:v>
+                  <c:v>787.40480000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>883.73387200000025</c:v>
+                  <c:v>818.90099200000009</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>936.75790432000031</c:v>
+                  <c:v>851.65703168000016</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>992.96337857920037</c:v>
+                  <c:v>885.72331294720016</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1052.5411812939524</c:v>
+                  <c:v>921.15224546508819</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1115.6936521715895</c:v>
+                  <c:v>957.99833528369174</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1182.635271301885</c:v>
+                  <c:v>996.31826869503948</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1253.5933875799983</c:v>
+                  <c:v>1036.1709994428411</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1328.8089908347984</c:v>
+                  <c:v>1077.6178394205547</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1230,37 +1231,37 @@
                   <c:v>3700</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3922</c:v>
+                  <c:v>3866</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4157.3200000000006</c:v>
+                  <c:v>4039.7200000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4406.7592000000004</c:v>
+                  <c:v>4221.5336000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4671.1647520000006</c:v>
+                  <c:v>4411.8332320000009</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4951.4346371200018</c:v>
+                  <c:v>4611.0311465600007</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5248.5207153472011</c:v>
+                  <c:v>4819.5604528192016</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5563.4319582680337</c:v>
+                  <c:v>5037.8762149525774</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5897.2378757641163</c:v>
+                  <c:v>5266.4566082125257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6251.0721483099642</c:v>
+                  <c:v>5505.8041378825819</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6626.1364772085617</c:v>
+                  <c:v>5756.4469246599338</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7023.7046658410763</c:v>
+                  <c:v>6018.9400601841025</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1467,40 +1468,40 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1140</c:v>
+                  <c:v>1863</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1208.4000000000001</c:v>
+                  <c:v>1974.7800000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1280.904</c:v>
+                  <c:v>2093.2668000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1357.7582400000001</c:v>
+                  <c:v>2218.8628080000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1439.2237344000002</c:v>
+                  <c:v>2351.9945764800004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1525.5771584640004</c:v>
+                  <c:v>2493.1142510688005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1617.1117879718404</c:v>
+                  <c:v>2642.7011061329285</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1714.1384952501508</c:v>
+                  <c:v>2801.2631725009046</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1816.98680496516</c:v>
+                  <c:v>2969.3389628509585</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1926.0060132630697</c:v>
+                  <c:v>3147.4993006220166</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2041.5663740588541</c:v>
+                  <c:v>3336.3492586593384</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2164.0603565023853</c:v>
+                  <c:v>3536.5302141788989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1888,13 +1889,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>62418.782429858955</c:v>
+                  <c:v>57255.202377270922</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>40825.257697367211</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19231.73296487546</c:v>
+                  <c:v>31428.700450493845</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4054,11 +4055,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4125,52 +4126,52 @@
         <v>1000</v>
       </c>
       <c r="C4" s="1">
-        <f>B4*1.06</f>
-        <v>1060</v>
+        <f>B4*1.04</f>
+        <v>1040</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:M4" si="0">C4*1.06</f>
-        <v>1123.6000000000001</v>
+        <f t="shared" ref="D4:M4" si="0">C4*1.04</f>
+        <v>1081.6000000000001</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>1191.0160000000003</v>
+        <v>1124.8640000000003</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>1262.4769600000004</v>
+        <v>1169.8585600000004</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>1338.2255776000004</v>
+        <v>1216.6529024000004</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="0"/>
-        <v>1418.5191122560004</v>
+        <v>1265.3190184960004</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="0"/>
-        <v>1503.6302589913605</v>
+        <v>1315.9317792358404</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="0"/>
-        <v>1593.8480745308423</v>
+        <v>1368.5690504052741</v>
       </c>
       <c r="K4" s="1">
         <f t="shared" si="0"/>
-        <v>1689.4789590026928</v>
+        <v>1423.311812421485</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" si="0"/>
-        <v>1790.8476965428545</v>
+        <v>1480.2442849183444</v>
       </c>
       <c r="M4" s="1">
         <f t="shared" si="0"/>
-        <v>1898.2985583354259</v>
+        <v>1539.4540563150783</v>
       </c>
       <c r="N4" s="6">
         <f>SUM(B4:M4)</f>
-        <v>16869.941197259181</v>
+        <v>15025.805464192024</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -4181,52 +4182,52 @@
         <v>1100</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" ref="C5:M5" si="1">B5*1.06</f>
-        <v>1166</v>
+        <f>B5*1.04</f>
+        <v>1144</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="1"/>
-        <v>1235.96</v>
+        <f t="shared" ref="D5:M5" si="1">C5*1.04</f>
+        <v>1189.76</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="1"/>
-        <v>1310.1176</v>
+        <v>1237.3504</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="1"/>
-        <v>1388.7246560000001</v>
+        <v>1286.8444160000001</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="1"/>
-        <v>1472.0481353600003</v>
+        <v>1338.3181926400002</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>1560.3710234816003</v>
+        <v>1391.8509203456003</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="1"/>
-        <v>1653.9932848904964</v>
+        <v>1447.5249571594245</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="1"/>
-        <v>1753.2328819839263</v>
+        <v>1505.4259554458015</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" si="1"/>
-        <v>1858.4268549029618</v>
+        <v>1565.6429936636337</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="1"/>
-        <v>1969.9324661971395</v>
+        <v>1628.2687134101791</v>
       </c>
       <c r="M5" s="1">
         <f t="shared" si="1"/>
-        <v>2088.128414168968</v>
+        <v>1693.3994619465864</v>
       </c>
       <c r="N5" s="6">
         <f t="shared" ref="N5:N20" si="2">SUM(B5:M5)</f>
-        <v>18556.935316985095</v>
+        <v>16528.386010611226</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -4237,52 +4238,52 @@
         <v>700</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" ref="C6:M6" si="3">B6*1.06</f>
-        <v>742</v>
+        <f>B6*1.04</f>
+        <v>728</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="3"/>
-        <v>786.5200000000001</v>
+        <f t="shared" ref="D6:M6" si="3">C6*1.04</f>
+        <v>757.12</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="3"/>
-        <v>833.71120000000019</v>
+        <v>787.40480000000002</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="3"/>
-        <v>883.73387200000025</v>
+        <v>818.90099200000009</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="3"/>
-        <v>936.75790432000031</v>
+        <v>851.65703168000016</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="3"/>
-        <v>992.96337857920037</v>
+        <v>885.72331294720016</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="3"/>
-        <v>1052.5411812939524</v>
+        <v>921.15224546508819</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>1115.6936521715895</v>
+        <v>957.99833528369174</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" si="3"/>
-        <v>1182.635271301885</v>
+        <v>996.31826869503948</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="3"/>
-        <v>1253.5933875799983</v>
+        <v>1036.1709994428411</v>
       </c>
       <c r="M6" s="1">
         <f t="shared" si="3"/>
-        <v>1328.8089908347984</v>
+        <v>1077.6178394205547</v>
       </c>
       <c r="N6" s="6">
         <f t="shared" si="2"/>
-        <v>11808.958838081424</v>
+        <v>10518.063824934414</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -4293,47 +4294,47 @@
         <v>900</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" ref="C7:M7" si="4">B7*1.06</f>
+        <f t="shared" ref="C7" si="4">B7*1.06</f>
         <v>954</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="D7" si="5">C7*1.06</f>
         <v>1011.24</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="E7" si="6">D7*1.06</f>
         <v>1071.9144000000001</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="F7" si="7">E7*1.06</f>
         <v>1136.2292640000003</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="G7" si="8">F7*1.06</f>
         <v>1204.4030198400003</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="H7" si="9">G7*1.06</f>
         <v>1276.6672010304003</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="I7" si="10">H7*1.06</f>
         <v>1353.2672330922244</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="J7" si="11">I7*1.06</f>
         <v>1434.463267077758</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="K7" si="12">J7*1.06</f>
         <v>1520.5310631024236</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="L7" si="13">K7*1.06</f>
         <v>1611.7629268885692</v>
       </c>
       <c r="M7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="M7" si="14">L7*1.06</f>
         <v>1708.4687025018834</v>
       </c>
       <c r="N7" s="6">
@@ -4350,52 +4351,52 @@
         <v>3700</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:N8" si="5">SUM(C4:C7)</f>
-        <v>3922</v>
+        <f t="shared" ref="C8:N8" si="15">SUM(C4:C7)</f>
+        <v>3866</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="5"/>
-        <v>4157.3200000000006</v>
+        <f t="shared" si="15"/>
+        <v>4039.7200000000003</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="5"/>
-        <v>4406.7592000000004</v>
+        <f t="shared" si="15"/>
+        <v>4221.5336000000007</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="5"/>
-        <v>4671.1647520000006</v>
+        <f t="shared" si="15"/>
+        <v>4411.8332320000009</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="5"/>
-        <v>4951.4346371200018</v>
+        <f t="shared" si="15"/>
+        <v>4611.0311465600007</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="5"/>
-        <v>5248.5207153472011</v>
+        <f t="shared" si="15"/>
+        <v>4819.5604528192016</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="5"/>
-        <v>5563.4319582680337</v>
+        <f t="shared" si="15"/>
+        <v>5037.8762149525774</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="5"/>
-        <v>5897.2378757641163</v>
+        <f t="shared" si="15"/>
+        <v>5266.4566082125257</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" si="5"/>
-        <v>6251.0721483099642</v>
+        <f t="shared" si="15"/>
+        <v>5505.8041378825819</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" si="5"/>
-        <v>6626.1364772085617</v>
+        <f t="shared" si="15"/>
+        <v>5756.4469246599338</v>
       </c>
       <c r="M8" s="1">
-        <f t="shared" si="5"/>
-        <v>7023.7046658410763</v>
+        <f t="shared" si="15"/>
+        <v>6018.9400601841025</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="5"/>
-        <v>62418.782429858955</v>
+        <f t="shared" si="15"/>
+        <v>57255.202377270922</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -4469,43 +4470,43 @@
         <v>530</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" ref="D11:M11" si="6">C11*1.06</f>
+        <f t="shared" ref="D11:M11" si="16">C11*1.06</f>
         <v>561.80000000000007</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>595.50800000000015</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>631.23848000000021</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>669.1127888000002</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>709.25955612800021</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>751.81512949568025</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>796.92403726542113</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>844.73947950134641</v>
       </c>
       <c r="L11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>895.42384827142723</v>
       </c>
       <c r="M11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>949.14927916771296</v>
       </c>
       <c r="N11" s="6">
@@ -4521,47 +4522,47 @@
         <v>600</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" ref="C12:M12" si="7">B12*1.06</f>
+        <f t="shared" ref="C12:M12" si="17">B12*1.06</f>
         <v>636</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>674.16000000000008</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>714.60960000000011</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>757.48617600000011</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>802.9353465600002</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>851.11146735360023</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>902.17815539481626</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>956.30884471850527</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>1013.6873754016157</v>
       </c>
       <c r="L12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>1074.5086179257128</v>
       </c>
       <c r="M12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>1138.9791350012556</v>
       </c>
       <c r="N12" s="6">
@@ -4577,47 +4578,47 @@
         <v>700</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" ref="C13:M13" si="8">B13*1.06</f>
+        <f t="shared" ref="C13:M13" si="18">B13*1.06</f>
         <v>742</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>786.5200000000001</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>833.71120000000019</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>883.73387200000025</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>936.75790432000031</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>992.96337857920037</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>1052.5411812939524</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>1115.6936521715895</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>1182.635271301885</v>
       </c>
       <c r="L13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>1253.5933875799983</v>
       </c>
       <c r="M13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>1328.8089908347984</v>
       </c>
       <c r="N13" s="6">
@@ -4633,51 +4634,51 @@
         <v>620</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" ref="C14" si="9">B14*1.06</f>
+        <f t="shared" ref="C14" si="19">B14*1.06</f>
         <v>657.2</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" ref="D14" si="10">C14*1.06</f>
+        <f t="shared" ref="D14" si="20">C14*1.06</f>
         <v>696.63200000000006</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" ref="E14" si="11">D14*1.06</f>
+        <f t="shared" ref="E14" si="21">D14*1.06</f>
         <v>738.42992000000015</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" ref="F14" si="12">E14*1.06</f>
+        <f t="shared" ref="F14" si="22">E14*1.06</f>
         <v>782.73571520000019</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" ref="G14" si="13">F14*1.06</f>
+        <f t="shared" ref="G14" si="23">F14*1.06</f>
         <v>829.69985811200024</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" ref="H14" si="14">G14*1.06</f>
+        <f t="shared" ref="H14" si="24">G14*1.06</f>
         <v>879.48184959872026</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" ref="I14" si="15">H14*1.06</f>
+        <f t="shared" ref="I14" si="25">H14*1.06</f>
         <v>932.25076057464355</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" ref="J14" si="16">I14*1.06</f>
+        <f t="shared" ref="J14" si="26">I14*1.06</f>
         <v>988.18580620912223</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" ref="K14" si="17">J14*1.06</f>
+        <f t="shared" ref="K14" si="27">J14*1.06</f>
         <v>1047.4769545816696</v>
       </c>
       <c r="L14" s="1">
-        <f t="shared" ref="L14" si="18">K14*1.06</f>
+        <f t="shared" ref="L14" si="28">K14*1.06</f>
         <v>1110.3255718565699</v>
       </c>
       <c r="M14" s="1">
-        <f t="shared" ref="M14" si="19">L14*1.06</f>
+        <f t="shared" ref="M14" si="29">L14*1.06</f>
         <v>1176.9451061679642</v>
       </c>
       <c r="N14" s="6">
-        <f t="shared" ref="N14" si="20">SUM(B14:M14)</f>
+        <f t="shared" ref="N14" si="30">SUM(B14:M14)</f>
         <v>10459.363542300691</v>
       </c>
     </row>
@@ -4690,51 +4691,51 @@
         <v>2420</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ref="C15" si="21">SUM(C11:C14)</f>
+        <f t="shared" ref="C15" si="31">SUM(C11:C14)</f>
         <v>2565.1999999999998</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" ref="D15" si="22">SUM(D11:D14)</f>
+        <f t="shared" ref="D15" si="32">SUM(D11:D14)</f>
         <v>2719.1120000000001</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" ref="E15" si="23">SUM(E11:E14)</f>
+        <f t="shared" ref="E15" si="33">SUM(E11:E14)</f>
         <v>2882.2587200000003</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" ref="F15" si="24">SUM(F11:F14)</f>
+        <f t="shared" ref="F15" si="34">SUM(F11:F14)</f>
         <v>3055.1942432000005</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" ref="G15" si="25">SUM(G11:G14)</f>
+        <f t="shared" ref="G15" si="35">SUM(G11:G14)</f>
         <v>3238.5058977920007</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" ref="H15" si="26">SUM(H11:H14)</f>
+        <f t="shared" ref="H15" si="36">SUM(H11:H14)</f>
         <v>3432.8162516595207</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" ref="I15" si="27">SUM(I11:I14)</f>
+        <f t="shared" ref="I15" si="37">SUM(I11:I14)</f>
         <v>3638.7852267590924</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" ref="J15" si="28">SUM(J11:J14)</f>
+        <f t="shared" ref="J15" si="38">SUM(J11:J14)</f>
         <v>3857.1123403646379</v>
       </c>
       <c r="K15" s="1">
-        <f t="shared" ref="K15" si="29">SUM(K11:K14)</f>
+        <f t="shared" ref="K15" si="39">SUM(K11:K14)</f>
         <v>4088.5390807865169</v>
       </c>
       <c r="L15" s="1">
-        <f t="shared" ref="L15" si="30">SUM(L11:L14)</f>
+        <f t="shared" ref="L15" si="40">SUM(L11:L14)</f>
         <v>4333.8514256337085</v>
       </c>
       <c r="M15" s="1">
-        <f t="shared" ref="M15" si="31">SUM(M11:M14)</f>
+        <f t="shared" ref="M15" si="41">SUM(M11:M14)</f>
         <v>4593.8825111717306</v>
       </c>
       <c r="N15" s="1">
-        <f t="shared" ref="N15" si="32">SUM(N11:N14)</f>
+        <f t="shared" ref="N15" si="42">SUM(N11:N14)</f>
         <v>40825.257697367211</v>
       </c>
     </row>
@@ -4802,55 +4803,55 @@
         <v>18</v>
       </c>
       <c r="B18" s="1">
-        <v>400</v>
+        <v>700</v>
       </c>
       <c r="C18" s="1">
         <f>B18*1.06</f>
-        <v>424</v>
+        <v>742</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" ref="D18:M18" si="33">C18*1.06</f>
-        <v>449.44</v>
+        <f t="shared" ref="D18:M18" si="43">C18*1.06</f>
+        <v>786.5200000000001</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="33"/>
-        <v>476.40640000000002</v>
+        <f t="shared" si="43"/>
+        <v>833.71120000000019</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="33"/>
-        <v>504.99078400000002</v>
+        <f t="shared" si="43"/>
+        <v>883.73387200000025</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="33"/>
-        <v>535.29023104000009</v>
+        <f t="shared" si="43"/>
+        <v>936.75790432000031</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="33"/>
-        <v>567.40764490240008</v>
+        <f t="shared" si="43"/>
+        <v>992.96337857920037</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="33"/>
-        <v>601.45210359654413</v>
+        <f t="shared" si="43"/>
+        <v>1052.5411812939524</v>
       </c>
       <c r="J18" s="1">
-        <f t="shared" si="33"/>
-        <v>637.53922981233677</v>
+        <f t="shared" si="43"/>
+        <v>1115.6936521715895</v>
       </c>
       <c r="K18" s="1">
-        <f t="shared" si="33"/>
-        <v>675.79158360107704</v>
+        <f t="shared" si="43"/>
+        <v>1182.635271301885</v>
       </c>
       <c r="L18" s="1">
-        <f t="shared" si="33"/>
-        <v>716.33907861714169</v>
+        <f t="shared" si="43"/>
+        <v>1253.5933875799983</v>
       </c>
       <c r="M18" s="1">
-        <f t="shared" si="33"/>
-        <v>759.31942333417021</v>
+        <f t="shared" si="43"/>
+        <v>1328.8089908347984</v>
       </c>
       <c r="N18" s="6">
         <f t="shared" si="2"/>
-        <v>6747.9764789036699</v>
+        <v>11808.958838081424</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -4858,55 +4859,55 @@
         <v>6</v>
       </c>
       <c r="B19" s="1">
-        <v>380</v>
+        <v>595</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" ref="C19:M19" si="34">B19*1.06</f>
-        <v>402.8</v>
+        <f t="shared" ref="C19:M19" si="44">B19*1.06</f>
+        <v>630.70000000000005</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="34"/>
-        <v>426.96800000000002</v>
+        <f t="shared" si="44"/>
+        <v>668.54200000000003</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="34"/>
-        <v>452.58608000000004</v>
+        <f t="shared" si="44"/>
+        <v>708.65452000000005</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="34"/>
-        <v>479.74124480000006</v>
+        <f t="shared" si="44"/>
+        <v>751.1737912000001</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="34"/>
-        <v>508.52571948800011</v>
+        <f t="shared" si="44"/>
+        <v>796.2442186720001</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="34"/>
-        <v>539.03726265728017</v>
+        <f t="shared" si="44"/>
+        <v>844.01887179232017</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="34"/>
-        <v>571.37949841671696</v>
+        <f t="shared" si="44"/>
+        <v>894.66000409985941</v>
       </c>
       <c r="J19" s="1">
-        <f t="shared" si="34"/>
-        <v>605.66226832172003</v>
+        <f t="shared" si="44"/>
+        <v>948.33960434585106</v>
       </c>
       <c r="K19" s="1">
-        <f t="shared" si="34"/>
-        <v>642.00200442102323</v>
+        <f t="shared" si="44"/>
+        <v>1005.2399806066022</v>
       </c>
       <c r="L19" s="1">
-        <f t="shared" si="34"/>
-        <v>680.52212468628466</v>
+        <f t="shared" si="44"/>
+        <v>1065.5543794429984</v>
       </c>
       <c r="M19" s="1">
-        <f t="shared" si="34"/>
-        <v>721.3534521674618</v>
+        <f t="shared" si="44"/>
+        <v>1129.4876422095783</v>
       </c>
       <c r="N19" s="6">
         <f t="shared" si="2"/>
-        <v>6410.5776549584871</v>
+        <v>10037.61501236921</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -4914,55 +4915,55 @@
         <v>7</v>
       </c>
       <c r="B20" s="1">
-        <v>360</v>
+        <v>568</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" ref="C20:M20" si="35">B20*1.06</f>
-        <v>381.6</v>
+        <f t="shared" ref="C20:M20" si="45">B20*1.06</f>
+        <v>602.08000000000004</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="35"/>
-        <v>404.49600000000004</v>
+        <f t="shared" si="45"/>
+        <v>638.20480000000009</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" si="35"/>
-        <v>428.76576000000006</v>
+        <f t="shared" si="45"/>
+        <v>676.49708800000008</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="35"/>
-        <v>454.4917056000001</v>
+        <f t="shared" si="45"/>
+        <v>717.08691328000009</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="35"/>
-        <v>481.76120793600012</v>
+        <f t="shared" si="45"/>
+        <v>760.1121280768001</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="35"/>
-        <v>510.66688041216014</v>
+        <f t="shared" si="45"/>
+        <v>805.71885576140812</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="35"/>
-        <v>541.30689323688978</v>
+        <f t="shared" si="45"/>
+        <v>854.0619871070927</v>
       </c>
       <c r="J20" s="1">
-        <f t="shared" si="35"/>
-        <v>573.78530683110318</v>
+        <f t="shared" si="45"/>
+        <v>905.30570633351829</v>
       </c>
       <c r="K20" s="1">
-        <f t="shared" si="35"/>
-        <v>608.21242524096942</v>
+        <f t="shared" si="45"/>
+        <v>959.62404871352942</v>
       </c>
       <c r="L20" s="1">
-        <f t="shared" si="35"/>
-        <v>644.70517075542762</v>
+        <f t="shared" si="45"/>
+        <v>1017.2014916363412</v>
       </c>
       <c r="M20" s="1">
-        <f t="shared" si="35"/>
-        <v>683.38748100075327</v>
+        <f t="shared" si="45"/>
+        <v>1078.2335811345217</v>
       </c>
       <c r="N20" s="6">
         <f t="shared" si="2"/>
-        <v>6073.1788310133034</v>
+        <v>9582.1266000432115</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -4971,55 +4972,55 @@
       </c>
       <c r="B21" s="1">
         <f>SUM(B18:B20)</f>
-        <v>1140</v>
+        <v>1863</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" ref="C21:N21" si="36">SUM(C18:C20)</f>
-        <v>1208.4000000000001</v>
+        <f t="shared" ref="C21:N21" si="46">SUM(C18:C20)</f>
+        <v>1974.7800000000002</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="36"/>
-        <v>1280.904</v>
+        <f t="shared" si="46"/>
+        <v>2093.2668000000003</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="36"/>
-        <v>1357.7582400000001</v>
+        <f t="shared" si="46"/>
+        <v>2218.8628080000003</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="36"/>
-        <v>1439.2237344000002</v>
+        <f t="shared" si="46"/>
+        <v>2351.9945764800004</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" si="36"/>
-        <v>1525.5771584640004</v>
+        <f t="shared" si="46"/>
+        <v>2493.1142510688005</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="36"/>
-        <v>1617.1117879718404</v>
+        <f t="shared" si="46"/>
+        <v>2642.7011061329285</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="36"/>
-        <v>1714.1384952501508</v>
+        <f t="shared" si="46"/>
+        <v>2801.2631725009046</v>
       </c>
       <c r="J21" s="1">
-        <f t="shared" si="36"/>
-        <v>1816.98680496516</v>
+        <f t="shared" si="46"/>
+        <v>2969.3389628509585</v>
       </c>
       <c r="K21" s="1">
-        <f t="shared" si="36"/>
-        <v>1926.0060132630697</v>
+        <f t="shared" si="46"/>
+        <v>3147.4993006220166</v>
       </c>
       <c r="L21" s="1">
-        <f t="shared" si="36"/>
-        <v>2041.5663740588541</v>
+        <f t="shared" si="46"/>
+        <v>3336.3492586593384</v>
       </c>
       <c r="M21" s="1">
-        <f t="shared" si="36"/>
-        <v>2164.0603565023853</v>
+        <f t="shared" si="46"/>
+        <v>3536.5302141788989</v>
       </c>
       <c r="N21" s="1">
-        <f t="shared" si="36"/>
-        <v>19231.73296487546</v>
+        <f t="shared" si="46"/>
+        <v>31428.700450493845</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -5073,52 +5074,52 @@
         <v>3700</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" ref="C25:M25" si="37">C8</f>
-        <v>3922</v>
+        <f t="shared" ref="C25:M25" si="47">C8</f>
+        <v>3866</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="37"/>
-        <v>4157.3200000000006</v>
+        <f t="shared" si="47"/>
+        <v>4039.7200000000003</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="37"/>
-        <v>4406.7592000000004</v>
+        <f t="shared" si="47"/>
+        <v>4221.5336000000007</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="37"/>
-        <v>4671.1647520000006</v>
+        <f t="shared" si="47"/>
+        <v>4411.8332320000009</v>
       </c>
       <c r="G25" s="1">
-        <f t="shared" si="37"/>
-        <v>4951.4346371200018</v>
+        <f t="shared" si="47"/>
+        <v>4611.0311465600007</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="37"/>
-        <v>5248.5207153472011</v>
+        <f t="shared" si="47"/>
+        <v>4819.5604528192016</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" si="37"/>
-        <v>5563.4319582680337</v>
+        <f t="shared" si="47"/>
+        <v>5037.8762149525774</v>
       </c>
       <c r="J25" s="1">
-        <f t="shared" si="37"/>
-        <v>5897.2378757641163</v>
+        <f t="shared" si="47"/>
+        <v>5266.4566082125257</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="37"/>
-        <v>6251.0721483099642</v>
+        <f t="shared" si="47"/>
+        <v>5505.8041378825819</v>
       </c>
       <c r="L25" s="1">
-        <f t="shared" si="37"/>
-        <v>6626.1364772085617</v>
+        <f t="shared" si="47"/>
+        <v>5756.4469246599338</v>
       </c>
       <c r="M25" s="1">
-        <f t="shared" si="37"/>
-        <v>7023.7046658410763</v>
+        <f t="shared" si="47"/>
+        <v>6018.9400601841025</v>
       </c>
       <c r="N25" s="6">
         <f>N8</f>
-        <v>62418.782429858955</v>
+        <v>57255.202377270922</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -5131,47 +5132,47 @@
         <v>2420</v>
       </c>
       <c r="C26" s="1">
-        <f t="shared" ref="C26:M26" si="38">C15</f>
+        <f t="shared" ref="C26:M26" si="48">C15</f>
         <v>2565.1999999999998</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="48"/>
         <v>2719.1120000000001</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="48"/>
         <v>2882.2587200000003</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="48"/>
         <v>3055.1942432000005</v>
       </c>
       <c r="G26" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="48"/>
         <v>3238.5058977920007</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="48"/>
         <v>3432.8162516595207</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="48"/>
         <v>3638.7852267590924</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="48"/>
         <v>3857.1123403646379</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="48"/>
         <v>4088.5390807865169</v>
       </c>
       <c r="L26" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="48"/>
         <v>4333.8514256337085</v>
       </c>
       <c r="M26" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="48"/>
         <v>4593.8825111717306</v>
       </c>
       <c r="N26" s="6">
@@ -5186,55 +5187,55 @@
       </c>
       <c r="B27" s="1">
         <f>B21</f>
-        <v>1140</v>
+        <v>1863</v>
       </c>
       <c r="C27" s="1">
-        <f t="shared" ref="C27:M27" si="39">C21</f>
-        <v>1208.4000000000001</v>
+        <f t="shared" ref="C27:M27" si="49">C21</f>
+        <v>1974.7800000000002</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="39"/>
-        <v>1280.904</v>
+        <f t="shared" si="49"/>
+        <v>2093.2668000000003</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" si="39"/>
-        <v>1357.7582400000001</v>
+        <f t="shared" si="49"/>
+        <v>2218.8628080000003</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="39"/>
-        <v>1439.2237344000002</v>
+        <f t="shared" si="49"/>
+        <v>2351.9945764800004</v>
       </c>
       <c r="G27" s="1">
-        <f t="shared" si="39"/>
-        <v>1525.5771584640004</v>
+        <f t="shared" si="49"/>
+        <v>2493.1142510688005</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="39"/>
-        <v>1617.1117879718404</v>
+        <f t="shared" si="49"/>
+        <v>2642.7011061329285</v>
       </c>
       <c r="I27" s="1">
-        <f t="shared" si="39"/>
-        <v>1714.1384952501508</v>
+        <f t="shared" si="49"/>
+        <v>2801.2631725009046</v>
       </c>
       <c r="J27" s="1">
-        <f t="shared" si="39"/>
-        <v>1816.98680496516</v>
+        <f t="shared" si="49"/>
+        <v>2969.3389628509585</v>
       </c>
       <c r="K27" s="1">
-        <f t="shared" si="39"/>
-        <v>1926.0060132630697</v>
+        <f t="shared" si="49"/>
+        <v>3147.4993006220166</v>
       </c>
       <c r="L27" s="1">
-        <f t="shared" si="39"/>
-        <v>2041.5663740588541</v>
+        <f t="shared" si="49"/>
+        <v>3336.3492586593384</v>
       </c>
       <c r="M27" s="1">
-        <f t="shared" si="39"/>
-        <v>2164.0603565023853</v>
+        <f t="shared" si="49"/>
+        <v>3536.5302141788989</v>
       </c>
       <c r="N27" s="6">
         <f>N21</f>
-        <v>19231.73296487546</v>
+        <v>31428.700450493845</v>
       </c>
     </row>
   </sheetData>
@@ -5248,10 +5249,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5303,23 +5306,23 @@
       </c>
       <c r="C3" s="6">
         <f>SUM(FcstMonthlyFY2018!B4:D4)</f>
-        <v>3183.6000000000004</v>
+        <v>3121.6000000000004</v>
       </c>
       <c r="D3" s="6">
         <f>SUM(FcstMonthlyFY2018!E4:G4)</f>
-        <v>3791.7185376000007</v>
+        <v>3511.3754624000012</v>
       </c>
       <c r="E3" s="6">
         <f>SUM(FcstMonthlyFY2018!H4:J4)</f>
-        <v>4515.9974457782037</v>
+        <v>3949.8198481371151</v>
       </c>
       <c r="F3" s="6">
         <f>SUM(FcstMonthlyFY2018!K4:M4)</f>
-        <v>5378.6252138809732</v>
+        <v>4443.0101536549082</v>
       </c>
       <c r="G3" s="6">
         <f>SUM(C3:F3)</f>
-        <v>16869.941197259177</v>
+        <v>15025.805464192024</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -5331,23 +5334,23 @@
       </c>
       <c r="C4" s="6">
         <f>SUM(FcstMonthlyFY2018!B5:D5)</f>
-        <v>3501.96</v>
+        <v>3433.76</v>
       </c>
       <c r="D4" s="6">
         <f>SUM(FcstMonthlyFY2018!E5:G5)</f>
-        <v>4170.8903913600006</v>
+        <v>3862.5130086400004</v>
       </c>
       <c r="E4" s="6">
         <f>SUM(FcstMonthlyFY2018!H5:J5)</f>
-        <v>4967.597190356023</v>
+        <v>4344.8018329508259</v>
       </c>
       <c r="F4" s="6">
         <f>SUM(FcstMonthlyFY2018!K5:M5)</f>
-        <v>5916.4877352690692</v>
+        <v>4887.3111690203996</v>
       </c>
       <c r="G4" s="6">
         <f t="shared" ref="G4:G7" si="0">SUM(C4:F4)</f>
-        <v>18556.935316985095</v>
+        <v>16528.386010611226</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -5359,23 +5362,23 @@
       </c>
       <c r="C5" s="6">
         <f>SUM(FcstMonthlyFY2018!B6:D6)</f>
-        <v>2228.52</v>
+        <v>2185.12</v>
       </c>
       <c r="D5" s="6">
         <f>SUM(FcstMonthlyFY2018!E6:G6)</f>
-        <v>2654.2029763200007</v>
+        <v>2457.9628236800004</v>
       </c>
       <c r="E5" s="6">
         <f>SUM(FcstMonthlyFY2018!H6:J6)</f>
-        <v>3161.1982120447419</v>
+        <v>2764.8738936959799</v>
       </c>
       <c r="F5" s="6">
         <f>SUM(FcstMonthlyFY2018!K6:M6)</f>
-        <v>3765.0376497166817</v>
+        <v>3110.107107558435</v>
       </c>
       <c r="G5" s="6">
         <f t="shared" si="0"/>
-        <v>11808.958838081424</v>
+        <v>10518.063824934416</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -5412,23 +5415,23 @@
       </c>
       <c r="C7" s="6">
         <f>SUM(FcstMonthlyFY2018!B8:D8)</f>
-        <v>11779.32</v>
+        <v>11605.720000000001</v>
       </c>
       <c r="D7" s="6">
         <f>SUM(FcstMonthlyFY2018!E8:G8)</f>
-        <v>14029.358589120002</v>
+        <v>13244.397978560002</v>
       </c>
       <c r="E7" s="6">
         <f>SUM(FcstMonthlyFY2018!H8:J8)</f>
-        <v>16709.190549379353</v>
+        <v>15123.893275984305</v>
       </c>
       <c r="F7" s="6">
         <f>SUM(FcstMonthlyFY2018!K8:M8)</f>
-        <v>19900.913291359604</v>
+        <v>17281.191122726617</v>
       </c>
       <c r="G7" s="6">
         <f t="shared" si="0"/>
-        <v>62418.782429858962</v>
+        <v>57255.202377270929</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -5623,23 +5626,23 @@
       </c>
       <c r="C17" s="6">
         <f>SUM(FcstMonthlyFY2018!B18:D18)</f>
-        <v>1273.44</v>
+        <v>2228.52</v>
       </c>
       <c r="D17" s="6">
         <f>SUM(FcstMonthlyFY2018!E18:G18)</f>
-        <v>1516.6874150400001</v>
+        <v>2654.2029763200007</v>
       </c>
       <c r="E17" s="6">
         <f>SUM(FcstMonthlyFY2018!H18:J18)</f>
-        <v>1806.3989783112809</v>
+        <v>3161.1982120447419</v>
       </c>
       <c r="F17" s="6">
         <f>SUM(FcstMonthlyFY2018!K18:M18)</f>
-        <v>2151.4500855523888</v>
+        <v>3765.0376497166817</v>
       </c>
       <c r="G17" s="6">
         <f>SUM(C17:F17)</f>
-        <v>6747.9764789036708</v>
+        <v>11808.958838081424</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -5651,23 +5654,23 @@
       </c>
       <c r="C18" s="6">
         <f>SUM(FcstMonthlyFY2018!B19:D19)</f>
-        <v>1209.768</v>
+        <v>1894.2420000000002</v>
       </c>
       <c r="D18" s="6">
         <f>SUM(FcstMonthlyFY2018!E19:G19)</f>
-        <v>1440.8530442880001</v>
+        <v>2256.0725298720004</v>
       </c>
       <c r="E18" s="6">
         <f>SUM(FcstMonthlyFY2018!H19:J19)</f>
-        <v>1716.079029395717</v>
+        <v>2687.0184802380309</v>
       </c>
       <c r="F18" s="6">
         <f>SUM(FcstMonthlyFY2018!K19:M19)</f>
-        <v>2043.8775812747699</v>
+        <v>3200.2820022591786</v>
       </c>
       <c r="G18" s="6">
         <f t="shared" ref="G18:G19" si="3">SUM(C18:F18)</f>
-        <v>6410.5776549584871</v>
+        <v>10037.61501236921</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -5679,23 +5682,23 @@
       </c>
       <c r="C19" s="6">
         <f>SUM(FcstMonthlyFY2018!B20:D20)</f>
-        <v>1146.096</v>
+        <v>1808.2847999999999</v>
       </c>
       <c r="D19" s="6">
         <f>SUM(FcstMonthlyFY2018!E20:G20)</f>
-        <v>1365.0186735360003</v>
+        <v>2153.6961293568002</v>
       </c>
       <c r="E19" s="6">
         <f>SUM(FcstMonthlyFY2018!H20:J20)</f>
-        <v>1625.759080480153</v>
+        <v>2565.0865492020189</v>
       </c>
       <c r="F19" s="6">
         <f>SUM(FcstMonthlyFY2018!K20:M20)</f>
-        <v>1936.3050769971503</v>
+        <v>3055.0591214843926</v>
       </c>
       <c r="G19" s="6">
         <f t="shared" si="3"/>
-        <v>6073.1788310133034</v>
+        <v>9582.1266000432115</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -5704,23 +5707,23 @@
       </c>
       <c r="C20" s="6">
         <f>SUM(C17:C19)</f>
-        <v>3629.3040000000001</v>
+        <v>5931.0468000000001</v>
       </c>
       <c r="D20" s="6">
         <f t="shared" ref="D20:F20" si="4">SUM(D17:D19)</f>
-        <v>4322.5591328640003</v>
+        <v>7063.9716355488017</v>
       </c>
       <c r="E20" s="6">
         <f t="shared" si="4"/>
-        <v>5148.2370881871511</v>
+        <v>8413.3032414847912</v>
       </c>
       <c r="F20" s="6">
         <f t="shared" si="4"/>
-        <v>6131.6327438243097</v>
+        <v>10020.378773460252</v>
       </c>
       <c r="G20" s="6">
         <f>SUM(G17:G19)</f>
-        <v>19231.73296487546</v>
+        <v>31428.700450493845</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5747,23 +5750,23 @@
       </c>
       <c r="C23" s="6">
         <f>C7</f>
-        <v>11779.32</v>
+        <v>11605.720000000001</v>
       </c>
       <c r="D23" s="6">
         <f>D7</f>
-        <v>14029.358589120002</v>
+        <v>13244.397978560002</v>
       </c>
       <c r="E23" s="6">
         <f>E7</f>
-        <v>16709.190549379353</v>
+        <v>15123.893275984305</v>
       </c>
       <c r="F23" s="6">
         <f>F7</f>
-        <v>19900.913291359604</v>
+        <v>17281.191122726617</v>
       </c>
       <c r="G23" s="6">
         <f>SUM(C23:F23)</f>
-        <v>62418.782429858962</v>
+        <v>57255.202377270929</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -5799,23 +5802,23 @@
       </c>
       <c r="C25" s="6">
         <f>C20</f>
-        <v>3629.3040000000001</v>
+        <v>5931.0468000000001</v>
       </c>
       <c r="D25" s="6">
         <f>D20</f>
-        <v>4322.5591328640003</v>
+        <v>7063.9716355488017</v>
       </c>
       <c r="E25" s="6">
         <f>E20</f>
-        <v>5148.2370881871511</v>
+        <v>8413.3032414847912</v>
       </c>
       <c r="F25" s="6">
         <f>F20</f>
-        <v>6131.6327438243097</v>
+        <v>10020.378773460252</v>
       </c>
       <c r="G25" s="6">
         <f t="shared" si="5"/>
-        <v>19231.73296487546</v>
+        <v>31428.700450493845</v>
       </c>
     </row>
   </sheetData>
@@ -5825,11 +5828,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="H2" sqref="H2:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5880,23 +5883,23 @@
       </c>
       <c r="C3" s="12">
         <f>SUM(FcstMonthlyFY2018!B4:D4)</f>
-        <v>3183.6000000000004</v>
+        <v>3121.6000000000004</v>
       </c>
       <c r="D3" s="12">
         <f>SUM(FcstMonthlyFY2018!E4:G4)</f>
-        <v>3791.7185376000007</v>
+        <v>3511.3754624000012</v>
       </c>
       <c r="E3" s="12">
         <f>SUM(FcstMonthlyFY2018!H4:J4)</f>
-        <v>4515.9974457782037</v>
+        <v>3949.8198481371151</v>
       </c>
       <c r="F3" s="12">
         <f>SUM(FcstMonthlyFY2018!K4:M4)</f>
-        <v>5378.6252138809732</v>
+        <v>4443.0101536549082</v>
       </c>
       <c r="G3" s="12">
         <f>SUM(C3:F3)</f>
-        <v>16869.941197259177</v>
+        <v>15025.805464192024</v>
       </c>
       <c r="H3" s="18" t="s">
         <v>30</v>
@@ -5911,23 +5914,23 @@
       </c>
       <c r="C4" s="12">
         <f>SUM(FcstMonthlyFY2018!B5:D5)</f>
-        <v>3501.96</v>
+        <v>3433.76</v>
       </c>
       <c r="D4" s="12">
         <f>SUM(FcstMonthlyFY2018!E5:G5)</f>
-        <v>4170.8903913600006</v>
+        <v>3862.5130086400004</v>
       </c>
       <c r="E4" s="12">
         <f>SUM(FcstMonthlyFY2018!H5:J5)</f>
-        <v>4967.597190356023</v>
+        <v>4344.8018329508259</v>
       </c>
       <c r="F4" s="12">
         <f>SUM(FcstMonthlyFY2018!K5:M5)</f>
-        <v>5916.4877352690692</v>
+        <v>4887.3111690203996</v>
       </c>
       <c r="G4" s="12">
         <f t="shared" ref="G4:G7" si="0">SUM(C4:F4)</f>
-        <v>18556.935316985095</v>
+        <v>16528.386010611226</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>30</v>
@@ -5942,23 +5945,23 @@
       </c>
       <c r="C5" s="12">
         <f>SUM(FcstMonthlyFY2018!B6:D6)</f>
-        <v>2228.52</v>
+        <v>2185.12</v>
       </c>
       <c r="D5" s="12">
         <f>SUM(FcstMonthlyFY2018!E6:G6)</f>
-        <v>2654.2029763200007</v>
+        <v>2457.9628236800004</v>
       </c>
       <c r="E5" s="12">
         <f>SUM(FcstMonthlyFY2018!H6:J6)</f>
-        <v>3161.1982120447419</v>
+        <v>2764.8738936959799</v>
       </c>
       <c r="F5" s="12">
         <f>SUM(FcstMonthlyFY2018!K6:M6)</f>
-        <v>3765.0376497166817</v>
+        <v>3110.107107558435</v>
       </c>
       <c r="G5" s="12">
         <f t="shared" si="0"/>
-        <v>11808.958838081424</v>
+        <v>10518.063824934416</v>
       </c>
       <c r="H5" s="18" t="s">
         <v>30</v>
@@ -6004,23 +6007,23 @@
       </c>
       <c r="C7" s="12">
         <f>SUM(FcstMonthlyFY2018!B8:D8)</f>
-        <v>11779.32</v>
+        <v>11605.720000000001</v>
       </c>
       <c r="D7" s="12">
         <f>SUM(FcstMonthlyFY2018!E8:G8)</f>
-        <v>14029.358589120002</v>
+        <v>13244.397978560002</v>
       </c>
       <c r="E7" s="12">
         <f>SUM(FcstMonthlyFY2018!H8:J8)</f>
-        <v>16709.190549379353</v>
+        <v>15123.893275984305</v>
       </c>
       <c r="F7" s="12">
         <f>SUM(FcstMonthlyFY2018!K8:M8)</f>
-        <v>19900.913291359604</v>
+        <v>17281.191122726617</v>
       </c>
       <c r="G7" s="12">
         <f t="shared" si="0"/>
-        <v>62418.782429858962</v>
+        <v>57255.202377270929</v>
       </c>
       <c r="H7" s="18" t="s">
         <v>30</v>
@@ -6033,11 +6036,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6045,9 +6048,10 @@
     <col min="1" max="1" width="12.140625" style="10" customWidth="1"/>
     <col min="2" max="2" width="39.5703125" customWidth="1"/>
     <col min="3" max="7" width="14" style="12" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>23</v>
       </c>
@@ -6055,7 +6059,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
@@ -6074,10 +6078,13 @@
       <c r="G2" s="14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -6102,10 +6109,13 @@
         <f>SUM(C3:F3)</f>
         <v>8434.9705986295885</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -6130,10 +6140,13 @@
         <f t="shared" ref="G4:G5" si="0">SUM(C4:F4)</f>
         <v>10121.964718355506</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -6158,10 +6171,13 @@
         <f t="shared" si="0"/>
         <v>11808.958838081424</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -6186,8 +6202,14 @@
         <f>SUM(C6:F6)</f>
         <v>10459.363542300691</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>10</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
@@ -6210,6 +6232,9 @@
       <c r="G7" s="12">
         <f t="shared" ref="G7" si="1">SUM(C7:F7)</f>
         <v>40825.257697367211</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -6218,11 +6243,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6230,9 +6255,10 @@
     <col min="1" max="1" width="12.140625" style="10" customWidth="1"/>
     <col min="2" max="2" width="39.5703125" customWidth="1"/>
     <col min="3" max="7" width="14" style="12" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>23</v>
       </c>
@@ -6240,7 +6266,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
@@ -6259,115 +6285,136 @@
       <c r="G2" s="14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="12">
         <f>SUM(FcstMonthlyFY2018!B18:D18)</f>
-        <v>1273.44</v>
+        <v>2228.52</v>
       </c>
       <c r="D3" s="12">
         <f>SUM(FcstMonthlyFY2018!E18:G18)</f>
-        <v>1516.6874150400001</v>
+        <v>2654.2029763200007</v>
       </c>
       <c r="E3" s="12">
         <f>SUM(FcstMonthlyFY2018!H18:J18)</f>
-        <v>1806.3989783112809</v>
+        <v>3161.1982120447419</v>
       </c>
       <c r="F3" s="12">
         <f>SUM(FcstMonthlyFY2018!K18:M18)</f>
-        <v>2151.4500855523888</v>
+        <v>3765.0376497166817</v>
       </c>
       <c r="G3" s="12">
         <f>SUM(C3:F3)</f>
-        <v>6747.9764789036708</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11808.958838081424</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="12">
         <f>SUM(FcstMonthlyFY2018!B19:D19)</f>
-        <v>1209.768</v>
+        <v>1894.2420000000002</v>
       </c>
       <c r="D4" s="12">
         <f>SUM(FcstMonthlyFY2018!E19:G19)</f>
-        <v>1440.8530442880001</v>
+        <v>2256.0725298720004</v>
       </c>
       <c r="E4" s="12">
         <f>SUM(FcstMonthlyFY2018!H19:J19)</f>
-        <v>1716.079029395717</v>
+        <v>2687.0184802380309</v>
       </c>
       <c r="F4" s="12">
         <f>SUM(FcstMonthlyFY2018!K19:M19)</f>
-        <v>2043.8775812747699</v>
+        <v>3200.2820022591786</v>
       </c>
       <c r="G4" s="12">
         <f t="shared" ref="G4:G5" si="0">SUM(C4:F4)</f>
-        <v>6410.5776549584871</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10037.61501236921</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="12">
         <f>SUM(FcstMonthlyFY2018!B20:D20)</f>
-        <v>1146.096</v>
+        <v>1808.2847999999999</v>
       </c>
       <c r="D5" s="12">
         <f>SUM(FcstMonthlyFY2018!E20:G20)</f>
-        <v>1365.0186735360003</v>
+        <v>2153.6961293568002</v>
       </c>
       <c r="E5" s="12">
         <f>SUM(FcstMonthlyFY2018!H20:J20)</f>
-        <v>1625.759080480153</v>
+        <v>2565.0865492020189</v>
       </c>
       <c r="F5" s="12">
         <f>SUM(FcstMonthlyFY2018!K20:M20)</f>
-        <v>1936.3050769971503</v>
+        <v>3055.0591214843926</v>
       </c>
       <c r="G5" s="12">
         <f t="shared" si="0"/>
-        <v>6073.1788310133034</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9582.1266000432115</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>14</v>
+      </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="12">
         <f>SUM(C3:C5)</f>
-        <v>3629.3040000000001</v>
+        <v>5931.0468000000001</v>
       </c>
       <c r="D6" s="12">
         <f t="shared" ref="D6:F6" si="1">SUM(D3:D5)</f>
-        <v>4322.5591328640003</v>
+        <v>7063.9716355488017</v>
       </c>
       <c r="E6" s="12">
         <f t="shared" si="1"/>
-        <v>5148.2370881871511</v>
+        <v>8413.3032414847912</v>
       </c>
       <c r="F6" s="12">
         <f t="shared" si="1"/>
-        <v>6131.6327438243097</v>
+        <v>10020.378773460252</v>
       </c>
       <c r="G6" s="12">
         <f>SUM(G3:G5)</f>
-        <v>19231.73296487546</v>
-      </c>
+        <v>31428.700450493845</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Database folder, all contents, copied from rev 04/25/2018 at 6:00PM
</commit_message>
<xml_diff>
--- a/database/Beezniss_Forecast_2018.xlsx
+++ b/database/Beezniss_Forecast_2018.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thor-from-Asgard\Desktop\beezniss\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D48D589E-8A28-4F42-980B-0ED11BE9A792}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FcstMonthlyFY2018" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <sheet name="FcstQtrMitochonFY2018" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_Sheet1A6N91" hidden="1">FcstMonthlyFY2018!$A$4:$N$7</definedName>
+    <definedName name="_xlcn.WorksheetConnection_Sheet1A6N9" hidden="1">FcstMonthlyFY2018!$A$4:$N$7</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,8 +39,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="ThisWorkbookDataModel" description="Data Model" type="5" refreshedVersion="6" minRefreshableVersion="5" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="ThisWorkbookDataModel" description="Data Model" type="5" refreshedVersion="6" minRefreshableVersion="5" background="1">
     <dbPr connection="Data Model Connection" command="Model" commandType="1"/>
     <olapPr sendLocale="1" rowDrillCount="1000"/>
     <extLst>
@@ -48,11 +49,11 @@
       </ext>
     </extLst>
   </connection>
-  <connection id="2" name="WorksheetConnection_Sheet1!$A$6:$N$9" type="102" refreshedVersion="6" minRefreshableVersion="5">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="WorksheetConnection_Sheet1!$A$6:$N$9" type="102" refreshedVersion="6" minRefreshableVersion="5">
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Sheet1A6N91"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Sheet1A6N9"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="31">
   <si>
     <t>Chocolate Chip Cookies</t>
   </si>
@@ -154,13 +155,13 @@
     <t>5</t>
   </si>
   <si>
-    <t>2018-03-30</t>
+    <t>2018-04-26</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -458,37 +459,37 @@
                   <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1060</c:v>
+                  <c:v>1040</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1123.6000000000001</c:v>
+                  <c:v>1081.6000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1191.0160000000003</c:v>
+                  <c:v>1124.8640000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1262.4769600000004</c:v>
+                  <c:v>1169.8585600000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1338.2255776000004</c:v>
+                  <c:v>1216.6529024000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1418.5191122560004</c:v>
+                  <c:v>1265.3190184960004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1503.6302589913605</c:v>
+                  <c:v>1315.9317792358404</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1593.8480745308423</c:v>
+                  <c:v>1368.5690504052741</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1689.4789590026928</c:v>
+                  <c:v>1423.311812421485</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1790.8476965428545</c:v>
+                  <c:v>1480.2442849183444</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1898.2985583354259</c:v>
+                  <c:v>1539.4540563150783</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -578,37 +579,37 @@
                   <c:v>1100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1166</c:v>
+                  <c:v>1144</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1235.96</c:v>
+                  <c:v>1189.76</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1310.1176</c:v>
+                  <c:v>1237.3504</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1388.7246560000001</c:v>
+                  <c:v>1286.8444160000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1472.0481353600003</c:v>
+                  <c:v>1338.3181926400002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1560.3710234816003</c:v>
+                  <c:v>1391.8509203456003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1653.9932848904964</c:v>
+                  <c:v>1447.5249571594245</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1753.2328819839263</c:v>
+                  <c:v>1505.4259554458015</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1858.4268549029618</c:v>
+                  <c:v>1565.6429936636337</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1969.9324661971395</c:v>
+                  <c:v>1628.2687134101791</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2088.128414168968</c:v>
+                  <c:v>1693.3994619465864</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -698,37 +699,37 @@
                   <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>742</c:v>
+                  <c:v>728</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>786.5200000000001</c:v>
+                  <c:v>757.12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>833.71120000000019</c:v>
+                  <c:v>787.40480000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>883.73387200000025</c:v>
+                  <c:v>818.90099200000009</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>936.75790432000031</c:v>
+                  <c:v>851.65703168000016</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>992.96337857920037</c:v>
+                  <c:v>885.72331294720016</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1052.5411812939524</c:v>
+                  <c:v>921.15224546508819</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1115.6936521715895</c:v>
+                  <c:v>957.99833528369174</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1182.635271301885</c:v>
+                  <c:v>996.31826869503948</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1253.5933875799983</c:v>
+                  <c:v>1036.1709994428411</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1328.8089908347984</c:v>
+                  <c:v>1077.6178394205547</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1230,37 +1231,37 @@
                   <c:v>3700</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3922</c:v>
+                  <c:v>3866</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4157.3200000000006</c:v>
+                  <c:v>4039.7200000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4406.7592000000004</c:v>
+                  <c:v>4221.5336000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4671.1647520000006</c:v>
+                  <c:v>4411.8332320000009</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4951.4346371200018</c:v>
+                  <c:v>4611.0311465600007</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5248.5207153472011</c:v>
+                  <c:v>4819.5604528192016</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5563.4319582680337</c:v>
+                  <c:v>5037.8762149525774</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5897.2378757641163</c:v>
+                  <c:v>5266.4566082125257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6251.0721483099642</c:v>
+                  <c:v>5505.8041378825819</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6626.1364772085617</c:v>
+                  <c:v>5756.4469246599338</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7023.7046658410763</c:v>
+                  <c:v>6018.9400601841025</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1467,40 +1468,40 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1140</c:v>
+                  <c:v>1863</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1208.4000000000001</c:v>
+                  <c:v>1974.7800000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1280.904</c:v>
+                  <c:v>2093.2668000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1357.7582400000001</c:v>
+                  <c:v>2218.8628080000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1439.2237344000002</c:v>
+                  <c:v>2351.9945764800004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1525.5771584640004</c:v>
+                  <c:v>2493.1142510688005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1617.1117879718404</c:v>
+                  <c:v>2642.7011061329285</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1714.1384952501508</c:v>
+                  <c:v>2801.2631725009046</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1816.98680496516</c:v>
+                  <c:v>2969.3389628509585</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1926.0060132630697</c:v>
+                  <c:v>3147.4993006220166</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2041.5663740588541</c:v>
+                  <c:v>3336.3492586593384</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2164.0603565023853</c:v>
+                  <c:v>3536.5302141788989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1888,13 +1889,13 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>62418.782429858955</c:v>
+                  <c:v>57255.202377270922</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>40825.257697367211</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19231.73296487546</c:v>
+                  <c:v>31428.700450493845</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4054,11 +4055,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4125,52 +4126,52 @@
         <v>1000</v>
       </c>
       <c r="C4" s="1">
-        <f>B4*1.06</f>
-        <v>1060</v>
+        <f>B4*1.04</f>
+        <v>1040</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:M4" si="0">C4*1.06</f>
-        <v>1123.6000000000001</v>
+        <f t="shared" ref="D4:M4" si="0">C4*1.04</f>
+        <v>1081.6000000000001</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>1191.0160000000003</v>
+        <v>1124.8640000000003</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>1262.4769600000004</v>
+        <v>1169.8585600000004</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>1338.2255776000004</v>
+        <v>1216.6529024000004</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="0"/>
-        <v>1418.5191122560004</v>
+        <v>1265.3190184960004</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="0"/>
-        <v>1503.6302589913605</v>
+        <v>1315.9317792358404</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="0"/>
-        <v>1593.8480745308423</v>
+        <v>1368.5690504052741</v>
       </c>
       <c r="K4" s="1">
         <f t="shared" si="0"/>
-        <v>1689.4789590026928</v>
+        <v>1423.311812421485</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" si="0"/>
-        <v>1790.8476965428545</v>
+        <v>1480.2442849183444</v>
       </c>
       <c r="M4" s="1">
         <f t="shared" si="0"/>
-        <v>1898.2985583354259</v>
+        <v>1539.4540563150783</v>
       </c>
       <c r="N4" s="6">
         <f>SUM(B4:M4)</f>
-        <v>16869.941197259181</v>
+        <v>15025.805464192024</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -4181,52 +4182,52 @@
         <v>1100</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" ref="C5:M5" si="1">B5*1.06</f>
-        <v>1166</v>
+        <f>B5*1.04</f>
+        <v>1144</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="1"/>
-        <v>1235.96</v>
+        <f t="shared" ref="D5:M5" si="1">C5*1.04</f>
+        <v>1189.76</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="1"/>
-        <v>1310.1176</v>
+        <v>1237.3504</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="1"/>
-        <v>1388.7246560000001</v>
+        <v>1286.8444160000001</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="1"/>
-        <v>1472.0481353600003</v>
+        <v>1338.3181926400002</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>1560.3710234816003</v>
+        <v>1391.8509203456003</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="1"/>
-        <v>1653.9932848904964</v>
+        <v>1447.5249571594245</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="1"/>
-        <v>1753.2328819839263</v>
+        <v>1505.4259554458015</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" si="1"/>
-        <v>1858.4268549029618</v>
+        <v>1565.6429936636337</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="1"/>
-        <v>1969.9324661971395</v>
+        <v>1628.2687134101791</v>
       </c>
       <c r="M5" s="1">
         <f t="shared" si="1"/>
-        <v>2088.128414168968</v>
+        <v>1693.3994619465864</v>
       </c>
       <c r="N5" s="6">
         <f t="shared" ref="N5:N20" si="2">SUM(B5:M5)</f>
-        <v>18556.935316985095</v>
+        <v>16528.386010611226</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -4237,52 +4238,52 @@
         <v>700</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" ref="C6:M6" si="3">B6*1.06</f>
-        <v>742</v>
+        <f>B6*1.04</f>
+        <v>728</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="3"/>
-        <v>786.5200000000001</v>
+        <f t="shared" ref="D6:M6" si="3">C6*1.04</f>
+        <v>757.12</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="3"/>
-        <v>833.71120000000019</v>
+        <v>787.40480000000002</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="3"/>
-        <v>883.73387200000025</v>
+        <v>818.90099200000009</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="3"/>
-        <v>936.75790432000031</v>
+        <v>851.65703168000016</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="3"/>
-        <v>992.96337857920037</v>
+        <v>885.72331294720016</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="3"/>
-        <v>1052.5411812939524</v>
+        <v>921.15224546508819</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>1115.6936521715895</v>
+        <v>957.99833528369174</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" si="3"/>
-        <v>1182.635271301885</v>
+        <v>996.31826869503948</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="3"/>
-        <v>1253.5933875799983</v>
+        <v>1036.1709994428411</v>
       </c>
       <c r="M6" s="1">
         <f t="shared" si="3"/>
-        <v>1328.8089908347984</v>
+        <v>1077.6178394205547</v>
       </c>
       <c r="N6" s="6">
         <f t="shared" si="2"/>
-        <v>11808.958838081424</v>
+        <v>10518.063824934414</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -4293,47 +4294,47 @@
         <v>900</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" ref="C7:M7" si="4">B7*1.06</f>
+        <f t="shared" ref="C7" si="4">B7*1.06</f>
         <v>954</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="D7" si="5">C7*1.06</f>
         <v>1011.24</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="E7" si="6">D7*1.06</f>
         <v>1071.9144000000001</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="F7" si="7">E7*1.06</f>
         <v>1136.2292640000003</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="G7" si="8">F7*1.06</f>
         <v>1204.4030198400003</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="H7" si="9">G7*1.06</f>
         <v>1276.6672010304003</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="I7" si="10">H7*1.06</f>
         <v>1353.2672330922244</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="J7" si="11">I7*1.06</f>
         <v>1434.463267077758</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="K7" si="12">J7*1.06</f>
         <v>1520.5310631024236</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="L7" si="13">K7*1.06</f>
         <v>1611.7629268885692</v>
       </c>
       <c r="M7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="M7" si="14">L7*1.06</f>
         <v>1708.4687025018834</v>
       </c>
       <c r="N7" s="6">
@@ -4350,52 +4351,52 @@
         <v>3700</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:N8" si="5">SUM(C4:C7)</f>
-        <v>3922</v>
+        <f t="shared" ref="C8:N8" si="15">SUM(C4:C7)</f>
+        <v>3866</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="5"/>
-        <v>4157.3200000000006</v>
+        <f t="shared" si="15"/>
+        <v>4039.7200000000003</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="5"/>
-        <v>4406.7592000000004</v>
+        <f t="shared" si="15"/>
+        <v>4221.5336000000007</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="5"/>
-        <v>4671.1647520000006</v>
+        <f t="shared" si="15"/>
+        <v>4411.8332320000009</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="5"/>
-        <v>4951.4346371200018</v>
+        <f t="shared" si="15"/>
+        <v>4611.0311465600007</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="5"/>
-        <v>5248.5207153472011</v>
+        <f t="shared" si="15"/>
+        <v>4819.5604528192016</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="5"/>
-        <v>5563.4319582680337</v>
+        <f t="shared" si="15"/>
+        <v>5037.8762149525774</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="5"/>
-        <v>5897.2378757641163</v>
+        <f t="shared" si="15"/>
+        <v>5266.4566082125257</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" si="5"/>
-        <v>6251.0721483099642</v>
+        <f t="shared" si="15"/>
+        <v>5505.8041378825819</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" si="5"/>
-        <v>6626.1364772085617</v>
+        <f t="shared" si="15"/>
+        <v>5756.4469246599338</v>
       </c>
       <c r="M8" s="1">
-        <f t="shared" si="5"/>
-        <v>7023.7046658410763</v>
+        <f t="shared" si="15"/>
+        <v>6018.9400601841025</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="5"/>
-        <v>62418.782429858955</v>
+        <f t="shared" si="15"/>
+        <v>57255.202377270922</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -4469,43 +4470,43 @@
         <v>530</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" ref="D11:M11" si="6">C11*1.06</f>
+        <f t="shared" ref="D11:M11" si="16">C11*1.06</f>
         <v>561.80000000000007</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>595.50800000000015</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>631.23848000000021</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>669.1127888000002</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>709.25955612800021</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>751.81512949568025</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>796.92403726542113</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>844.73947950134641</v>
       </c>
       <c r="L11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>895.42384827142723</v>
       </c>
       <c r="M11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>949.14927916771296</v>
       </c>
       <c r="N11" s="6">
@@ -4521,47 +4522,47 @@
         <v>600</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" ref="C12:M12" si="7">B12*1.06</f>
+        <f t="shared" ref="C12:M12" si="17">B12*1.06</f>
         <v>636</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>674.16000000000008</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>714.60960000000011</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>757.48617600000011</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>802.9353465600002</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>851.11146735360023</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>902.17815539481626</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>956.30884471850527</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>1013.6873754016157</v>
       </c>
       <c r="L12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>1074.5086179257128</v>
       </c>
       <c r="M12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>1138.9791350012556</v>
       </c>
       <c r="N12" s="6">
@@ -4577,47 +4578,47 @@
         <v>700</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" ref="C13:M13" si="8">B13*1.06</f>
+        <f t="shared" ref="C13:M13" si="18">B13*1.06</f>
         <v>742</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>786.5200000000001</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>833.71120000000019</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>883.73387200000025</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>936.75790432000031</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>992.96337857920037</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>1052.5411812939524</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>1115.6936521715895</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>1182.635271301885</v>
       </c>
       <c r="L13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>1253.5933875799983</v>
       </c>
       <c r="M13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>1328.8089908347984</v>
       </c>
       <c r="N13" s="6">
@@ -4633,51 +4634,51 @@
         <v>620</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" ref="C14" si="9">B14*1.06</f>
+        <f t="shared" ref="C14" si="19">B14*1.06</f>
         <v>657.2</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" ref="D14" si="10">C14*1.06</f>
+        <f t="shared" ref="D14" si="20">C14*1.06</f>
         <v>696.63200000000006</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" ref="E14" si="11">D14*1.06</f>
+        <f t="shared" ref="E14" si="21">D14*1.06</f>
         <v>738.42992000000015</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" ref="F14" si="12">E14*1.06</f>
+        <f t="shared" ref="F14" si="22">E14*1.06</f>
         <v>782.73571520000019</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" ref="G14" si="13">F14*1.06</f>
+        <f t="shared" ref="G14" si="23">F14*1.06</f>
         <v>829.69985811200024</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" ref="H14" si="14">G14*1.06</f>
+        <f t="shared" ref="H14" si="24">G14*1.06</f>
         <v>879.48184959872026</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" ref="I14" si="15">H14*1.06</f>
+        <f t="shared" ref="I14" si="25">H14*1.06</f>
         <v>932.25076057464355</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" ref="J14" si="16">I14*1.06</f>
+        <f t="shared" ref="J14" si="26">I14*1.06</f>
         <v>988.18580620912223</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" ref="K14" si="17">J14*1.06</f>
+        <f t="shared" ref="K14" si="27">J14*1.06</f>
         <v>1047.4769545816696</v>
       </c>
       <c r="L14" s="1">
-        <f t="shared" ref="L14" si="18">K14*1.06</f>
+        <f t="shared" ref="L14" si="28">K14*1.06</f>
         <v>1110.3255718565699</v>
       </c>
       <c r="M14" s="1">
-        <f t="shared" ref="M14" si="19">L14*1.06</f>
+        <f t="shared" ref="M14" si="29">L14*1.06</f>
         <v>1176.9451061679642</v>
       </c>
       <c r="N14" s="6">
-        <f t="shared" ref="N14" si="20">SUM(B14:M14)</f>
+        <f t="shared" ref="N14" si="30">SUM(B14:M14)</f>
         <v>10459.363542300691</v>
       </c>
     </row>
@@ -4690,51 +4691,51 @@
         <v>2420</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ref="C15" si="21">SUM(C11:C14)</f>
+        <f t="shared" ref="C15" si="31">SUM(C11:C14)</f>
         <v>2565.1999999999998</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" ref="D15" si="22">SUM(D11:D14)</f>
+        <f t="shared" ref="D15" si="32">SUM(D11:D14)</f>
         <v>2719.1120000000001</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" ref="E15" si="23">SUM(E11:E14)</f>
+        <f t="shared" ref="E15" si="33">SUM(E11:E14)</f>
         <v>2882.2587200000003</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" ref="F15" si="24">SUM(F11:F14)</f>
+        <f t="shared" ref="F15" si="34">SUM(F11:F14)</f>
         <v>3055.1942432000005</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" ref="G15" si="25">SUM(G11:G14)</f>
+        <f t="shared" ref="G15" si="35">SUM(G11:G14)</f>
         <v>3238.5058977920007</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" ref="H15" si="26">SUM(H11:H14)</f>
+        <f t="shared" ref="H15" si="36">SUM(H11:H14)</f>
         <v>3432.8162516595207</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" ref="I15" si="27">SUM(I11:I14)</f>
+        <f t="shared" ref="I15" si="37">SUM(I11:I14)</f>
         <v>3638.7852267590924</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" ref="J15" si="28">SUM(J11:J14)</f>
+        <f t="shared" ref="J15" si="38">SUM(J11:J14)</f>
         <v>3857.1123403646379</v>
       </c>
       <c r="K15" s="1">
-        <f t="shared" ref="K15" si="29">SUM(K11:K14)</f>
+        <f t="shared" ref="K15" si="39">SUM(K11:K14)</f>
         <v>4088.5390807865169</v>
       </c>
       <c r="L15" s="1">
-        <f t="shared" ref="L15" si="30">SUM(L11:L14)</f>
+        <f t="shared" ref="L15" si="40">SUM(L11:L14)</f>
         <v>4333.8514256337085</v>
       </c>
       <c r="M15" s="1">
-        <f t="shared" ref="M15" si="31">SUM(M11:M14)</f>
+        <f t="shared" ref="M15" si="41">SUM(M11:M14)</f>
         <v>4593.8825111717306</v>
       </c>
       <c r="N15" s="1">
-        <f t="shared" ref="N15" si="32">SUM(N11:N14)</f>
+        <f t="shared" ref="N15" si="42">SUM(N11:N14)</f>
         <v>40825.257697367211</v>
       </c>
     </row>
@@ -4802,55 +4803,55 @@
         <v>18</v>
       </c>
       <c r="B18" s="1">
-        <v>400</v>
+        <v>700</v>
       </c>
       <c r="C18" s="1">
         <f>B18*1.06</f>
-        <v>424</v>
+        <v>742</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" ref="D18:M18" si="33">C18*1.06</f>
-        <v>449.44</v>
+        <f t="shared" ref="D18:M18" si="43">C18*1.06</f>
+        <v>786.5200000000001</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="33"/>
-        <v>476.40640000000002</v>
+        <f t="shared" si="43"/>
+        <v>833.71120000000019</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="33"/>
-        <v>504.99078400000002</v>
+        <f t="shared" si="43"/>
+        <v>883.73387200000025</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="33"/>
-        <v>535.29023104000009</v>
+        <f t="shared" si="43"/>
+        <v>936.75790432000031</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="33"/>
-        <v>567.40764490240008</v>
+        <f t="shared" si="43"/>
+        <v>992.96337857920037</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="33"/>
-        <v>601.45210359654413</v>
+        <f t="shared" si="43"/>
+        <v>1052.5411812939524</v>
       </c>
       <c r="J18" s="1">
-        <f t="shared" si="33"/>
-        <v>637.53922981233677</v>
+        <f t="shared" si="43"/>
+        <v>1115.6936521715895</v>
       </c>
       <c r="K18" s="1">
-        <f t="shared" si="33"/>
-        <v>675.79158360107704</v>
+        <f t="shared" si="43"/>
+        <v>1182.635271301885</v>
       </c>
       <c r="L18" s="1">
-        <f t="shared" si="33"/>
-        <v>716.33907861714169</v>
+        <f t="shared" si="43"/>
+        <v>1253.5933875799983</v>
       </c>
       <c r="M18" s="1">
-        <f t="shared" si="33"/>
-        <v>759.31942333417021</v>
+        <f t="shared" si="43"/>
+        <v>1328.8089908347984</v>
       </c>
       <c r="N18" s="6">
         <f t="shared" si="2"/>
-        <v>6747.9764789036699</v>
+        <v>11808.958838081424</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -4858,55 +4859,55 @@
         <v>6</v>
       </c>
       <c r="B19" s="1">
-        <v>380</v>
+        <v>595</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" ref="C19:M19" si="34">B19*1.06</f>
-        <v>402.8</v>
+        <f t="shared" ref="C19:M19" si="44">B19*1.06</f>
+        <v>630.70000000000005</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="34"/>
-        <v>426.96800000000002</v>
+        <f t="shared" si="44"/>
+        <v>668.54200000000003</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="34"/>
-        <v>452.58608000000004</v>
+        <f t="shared" si="44"/>
+        <v>708.65452000000005</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="34"/>
-        <v>479.74124480000006</v>
+        <f t="shared" si="44"/>
+        <v>751.1737912000001</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="34"/>
-        <v>508.52571948800011</v>
+        <f t="shared" si="44"/>
+        <v>796.2442186720001</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="34"/>
-        <v>539.03726265728017</v>
+        <f t="shared" si="44"/>
+        <v>844.01887179232017</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="34"/>
-        <v>571.37949841671696</v>
+        <f t="shared" si="44"/>
+        <v>894.66000409985941</v>
       </c>
       <c r="J19" s="1">
-        <f t="shared" si="34"/>
-        <v>605.66226832172003</v>
+        <f t="shared" si="44"/>
+        <v>948.33960434585106</v>
       </c>
       <c r="K19" s="1">
-        <f t="shared" si="34"/>
-        <v>642.00200442102323</v>
+        <f t="shared" si="44"/>
+        <v>1005.2399806066022</v>
       </c>
       <c r="L19" s="1">
-        <f t="shared" si="34"/>
-        <v>680.52212468628466</v>
+        <f t="shared" si="44"/>
+        <v>1065.5543794429984</v>
       </c>
       <c r="M19" s="1">
-        <f t="shared" si="34"/>
-        <v>721.3534521674618</v>
+        <f t="shared" si="44"/>
+        <v>1129.4876422095783</v>
       </c>
       <c r="N19" s="6">
         <f t="shared" si="2"/>
-        <v>6410.5776549584871</v>
+        <v>10037.61501236921</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -4914,55 +4915,55 @@
         <v>7</v>
       </c>
       <c r="B20" s="1">
-        <v>360</v>
+        <v>568</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" ref="C20:M20" si="35">B20*1.06</f>
-        <v>381.6</v>
+        <f t="shared" ref="C20:M20" si="45">B20*1.06</f>
+        <v>602.08000000000004</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="35"/>
-        <v>404.49600000000004</v>
+        <f t="shared" si="45"/>
+        <v>638.20480000000009</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" si="35"/>
-        <v>428.76576000000006</v>
+        <f t="shared" si="45"/>
+        <v>676.49708800000008</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="35"/>
-        <v>454.4917056000001</v>
+        <f t="shared" si="45"/>
+        <v>717.08691328000009</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="35"/>
-        <v>481.76120793600012</v>
+        <f t="shared" si="45"/>
+        <v>760.1121280768001</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="35"/>
-        <v>510.66688041216014</v>
+        <f t="shared" si="45"/>
+        <v>805.71885576140812</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="35"/>
-        <v>541.30689323688978</v>
+        <f t="shared" si="45"/>
+        <v>854.0619871070927</v>
       </c>
       <c r="J20" s="1">
-        <f t="shared" si="35"/>
-        <v>573.78530683110318</v>
+        <f t="shared" si="45"/>
+        <v>905.30570633351829</v>
       </c>
       <c r="K20" s="1">
-        <f t="shared" si="35"/>
-        <v>608.21242524096942</v>
+        <f t="shared" si="45"/>
+        <v>959.62404871352942</v>
       </c>
       <c r="L20" s="1">
-        <f t="shared" si="35"/>
-        <v>644.70517075542762</v>
+        <f t="shared" si="45"/>
+        <v>1017.2014916363412</v>
       </c>
       <c r="M20" s="1">
-        <f t="shared" si="35"/>
-        <v>683.38748100075327</v>
+        <f t="shared" si="45"/>
+        <v>1078.2335811345217</v>
       </c>
       <c r="N20" s="6">
         <f t="shared" si="2"/>
-        <v>6073.1788310133034</v>
+        <v>9582.1266000432115</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -4971,55 +4972,55 @@
       </c>
       <c r="B21" s="1">
         <f>SUM(B18:B20)</f>
-        <v>1140</v>
+        <v>1863</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" ref="C21:N21" si="36">SUM(C18:C20)</f>
-        <v>1208.4000000000001</v>
+        <f t="shared" ref="C21:N21" si="46">SUM(C18:C20)</f>
+        <v>1974.7800000000002</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="36"/>
-        <v>1280.904</v>
+        <f t="shared" si="46"/>
+        <v>2093.2668000000003</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="36"/>
-        <v>1357.7582400000001</v>
+        <f t="shared" si="46"/>
+        <v>2218.8628080000003</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="36"/>
-        <v>1439.2237344000002</v>
+        <f t="shared" si="46"/>
+        <v>2351.9945764800004</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" si="36"/>
-        <v>1525.5771584640004</v>
+        <f t="shared" si="46"/>
+        <v>2493.1142510688005</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="36"/>
-        <v>1617.1117879718404</v>
+        <f t="shared" si="46"/>
+        <v>2642.7011061329285</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="36"/>
-        <v>1714.1384952501508</v>
+        <f t="shared" si="46"/>
+        <v>2801.2631725009046</v>
       </c>
       <c r="J21" s="1">
-        <f t="shared" si="36"/>
-        <v>1816.98680496516</v>
+        <f t="shared" si="46"/>
+        <v>2969.3389628509585</v>
       </c>
       <c r="K21" s="1">
-        <f t="shared" si="36"/>
-        <v>1926.0060132630697</v>
+        <f t="shared" si="46"/>
+        <v>3147.4993006220166</v>
       </c>
       <c r="L21" s="1">
-        <f t="shared" si="36"/>
-        <v>2041.5663740588541</v>
+        <f t="shared" si="46"/>
+        <v>3336.3492586593384</v>
       </c>
       <c r="M21" s="1">
-        <f t="shared" si="36"/>
-        <v>2164.0603565023853</v>
+        <f t="shared" si="46"/>
+        <v>3536.5302141788989</v>
       </c>
       <c r="N21" s="1">
-        <f t="shared" si="36"/>
-        <v>19231.73296487546</v>
+        <f t="shared" si="46"/>
+        <v>31428.700450493845</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -5073,52 +5074,52 @@
         <v>3700</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" ref="C25:M25" si="37">C8</f>
-        <v>3922</v>
+        <f t="shared" ref="C25:M25" si="47">C8</f>
+        <v>3866</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="37"/>
-        <v>4157.3200000000006</v>
+        <f t="shared" si="47"/>
+        <v>4039.7200000000003</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="37"/>
-        <v>4406.7592000000004</v>
+        <f t="shared" si="47"/>
+        <v>4221.5336000000007</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="37"/>
-        <v>4671.1647520000006</v>
+        <f t="shared" si="47"/>
+        <v>4411.8332320000009</v>
       </c>
       <c r="G25" s="1">
-        <f t="shared" si="37"/>
-        <v>4951.4346371200018</v>
+        <f t="shared" si="47"/>
+        <v>4611.0311465600007</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="37"/>
-        <v>5248.5207153472011</v>
+        <f t="shared" si="47"/>
+        <v>4819.5604528192016</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" si="37"/>
-        <v>5563.4319582680337</v>
+        <f t="shared" si="47"/>
+        <v>5037.8762149525774</v>
       </c>
       <c r="J25" s="1">
-        <f t="shared" si="37"/>
-        <v>5897.2378757641163</v>
+        <f t="shared" si="47"/>
+        <v>5266.4566082125257</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="37"/>
-        <v>6251.0721483099642</v>
+        <f t="shared" si="47"/>
+        <v>5505.8041378825819</v>
       </c>
       <c r="L25" s="1">
-        <f t="shared" si="37"/>
-        <v>6626.1364772085617</v>
+        <f t="shared" si="47"/>
+        <v>5756.4469246599338</v>
       </c>
       <c r="M25" s="1">
-        <f t="shared" si="37"/>
-        <v>7023.7046658410763</v>
+        <f t="shared" si="47"/>
+        <v>6018.9400601841025</v>
       </c>
       <c r="N25" s="6">
         <f>N8</f>
-        <v>62418.782429858955</v>
+        <v>57255.202377270922</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -5131,47 +5132,47 @@
         <v>2420</v>
       </c>
       <c r="C26" s="1">
-        <f t="shared" ref="C26:M26" si="38">C15</f>
+        <f t="shared" ref="C26:M26" si="48">C15</f>
         <v>2565.1999999999998</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="48"/>
         <v>2719.1120000000001</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="48"/>
         <v>2882.2587200000003</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="48"/>
         <v>3055.1942432000005</v>
       </c>
       <c r="G26" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="48"/>
         <v>3238.5058977920007</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="48"/>
         <v>3432.8162516595207</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="48"/>
         <v>3638.7852267590924</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="48"/>
         <v>3857.1123403646379</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="48"/>
         <v>4088.5390807865169</v>
       </c>
       <c r="L26" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="48"/>
         <v>4333.8514256337085</v>
       </c>
       <c r="M26" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="48"/>
         <v>4593.8825111717306</v>
       </c>
       <c r="N26" s="6">
@@ -5186,55 +5187,55 @@
       </c>
       <c r="B27" s="1">
         <f>B21</f>
-        <v>1140</v>
+        <v>1863</v>
       </c>
       <c r="C27" s="1">
-        <f t="shared" ref="C27:M27" si="39">C21</f>
-        <v>1208.4000000000001</v>
+        <f t="shared" ref="C27:M27" si="49">C21</f>
+        <v>1974.7800000000002</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="39"/>
-        <v>1280.904</v>
+        <f t="shared" si="49"/>
+        <v>2093.2668000000003</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" si="39"/>
-        <v>1357.7582400000001</v>
+        <f t="shared" si="49"/>
+        <v>2218.8628080000003</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="39"/>
-        <v>1439.2237344000002</v>
+        <f t="shared" si="49"/>
+        <v>2351.9945764800004</v>
       </c>
       <c r="G27" s="1">
-        <f t="shared" si="39"/>
-        <v>1525.5771584640004</v>
+        <f t="shared" si="49"/>
+        <v>2493.1142510688005</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="39"/>
-        <v>1617.1117879718404</v>
+        <f t="shared" si="49"/>
+        <v>2642.7011061329285</v>
       </c>
       <c r="I27" s="1">
-        <f t="shared" si="39"/>
-        <v>1714.1384952501508</v>
+        <f t="shared" si="49"/>
+        <v>2801.2631725009046</v>
       </c>
       <c r="J27" s="1">
-        <f t="shared" si="39"/>
-        <v>1816.98680496516</v>
+        <f t="shared" si="49"/>
+        <v>2969.3389628509585</v>
       </c>
       <c r="K27" s="1">
-        <f t="shared" si="39"/>
-        <v>1926.0060132630697</v>
+        <f t="shared" si="49"/>
+        <v>3147.4993006220166</v>
       </c>
       <c r="L27" s="1">
-        <f t="shared" si="39"/>
-        <v>2041.5663740588541</v>
+        <f t="shared" si="49"/>
+        <v>3336.3492586593384</v>
       </c>
       <c r="M27" s="1">
-        <f t="shared" si="39"/>
-        <v>2164.0603565023853</v>
+        <f t="shared" si="49"/>
+        <v>3536.5302141788989</v>
       </c>
       <c r="N27" s="6">
         <f>N21</f>
-        <v>19231.73296487546</v>
+        <v>31428.700450493845</v>
       </c>
     </row>
   </sheetData>
@@ -5248,10 +5249,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5303,23 +5306,23 @@
       </c>
       <c r="C3" s="6">
         <f>SUM(FcstMonthlyFY2018!B4:D4)</f>
-        <v>3183.6000000000004</v>
+        <v>3121.6000000000004</v>
       </c>
       <c r="D3" s="6">
         <f>SUM(FcstMonthlyFY2018!E4:G4)</f>
-        <v>3791.7185376000007</v>
+        <v>3511.3754624000012</v>
       </c>
       <c r="E3" s="6">
         <f>SUM(FcstMonthlyFY2018!H4:J4)</f>
-        <v>4515.9974457782037</v>
+        <v>3949.8198481371151</v>
       </c>
       <c r="F3" s="6">
         <f>SUM(FcstMonthlyFY2018!K4:M4)</f>
-        <v>5378.6252138809732</v>
+        <v>4443.0101536549082</v>
       </c>
       <c r="G3" s="6">
         <f>SUM(C3:F3)</f>
-        <v>16869.941197259177</v>
+        <v>15025.805464192024</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -5331,23 +5334,23 @@
       </c>
       <c r="C4" s="6">
         <f>SUM(FcstMonthlyFY2018!B5:D5)</f>
-        <v>3501.96</v>
+        <v>3433.76</v>
       </c>
       <c r="D4" s="6">
         <f>SUM(FcstMonthlyFY2018!E5:G5)</f>
-        <v>4170.8903913600006</v>
+        <v>3862.5130086400004</v>
       </c>
       <c r="E4" s="6">
         <f>SUM(FcstMonthlyFY2018!H5:J5)</f>
-        <v>4967.597190356023</v>
+        <v>4344.8018329508259</v>
       </c>
       <c r="F4" s="6">
         <f>SUM(FcstMonthlyFY2018!K5:M5)</f>
-        <v>5916.4877352690692</v>
+        <v>4887.3111690203996</v>
       </c>
       <c r="G4" s="6">
         <f t="shared" ref="G4:G7" si="0">SUM(C4:F4)</f>
-        <v>18556.935316985095</v>
+        <v>16528.386010611226</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -5359,23 +5362,23 @@
       </c>
       <c r="C5" s="6">
         <f>SUM(FcstMonthlyFY2018!B6:D6)</f>
-        <v>2228.52</v>
+        <v>2185.12</v>
       </c>
       <c r="D5" s="6">
         <f>SUM(FcstMonthlyFY2018!E6:G6)</f>
-        <v>2654.2029763200007</v>
+        <v>2457.9628236800004</v>
       </c>
       <c r="E5" s="6">
         <f>SUM(FcstMonthlyFY2018!H6:J6)</f>
-        <v>3161.1982120447419</v>
+        <v>2764.8738936959799</v>
       </c>
       <c r="F5" s="6">
         <f>SUM(FcstMonthlyFY2018!K6:M6)</f>
-        <v>3765.0376497166817</v>
+        <v>3110.107107558435</v>
       </c>
       <c r="G5" s="6">
         <f t="shared" si="0"/>
-        <v>11808.958838081424</v>
+        <v>10518.063824934416</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -5412,23 +5415,23 @@
       </c>
       <c r="C7" s="6">
         <f>SUM(FcstMonthlyFY2018!B8:D8)</f>
-        <v>11779.32</v>
+        <v>11605.720000000001</v>
       </c>
       <c r="D7" s="6">
         <f>SUM(FcstMonthlyFY2018!E8:G8)</f>
-        <v>14029.358589120002</v>
+        <v>13244.397978560002</v>
       </c>
       <c r="E7" s="6">
         <f>SUM(FcstMonthlyFY2018!H8:J8)</f>
-        <v>16709.190549379353</v>
+        <v>15123.893275984305</v>
       </c>
       <c r="F7" s="6">
         <f>SUM(FcstMonthlyFY2018!K8:M8)</f>
-        <v>19900.913291359604</v>
+        <v>17281.191122726617</v>
       </c>
       <c r="G7" s="6">
         <f t="shared" si="0"/>
-        <v>62418.782429858962</v>
+        <v>57255.202377270929</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -5623,23 +5626,23 @@
       </c>
       <c r="C17" s="6">
         <f>SUM(FcstMonthlyFY2018!B18:D18)</f>
-        <v>1273.44</v>
+        <v>2228.52</v>
       </c>
       <c r="D17" s="6">
         <f>SUM(FcstMonthlyFY2018!E18:G18)</f>
-        <v>1516.6874150400001</v>
+        <v>2654.2029763200007</v>
       </c>
       <c r="E17" s="6">
         <f>SUM(FcstMonthlyFY2018!H18:J18)</f>
-        <v>1806.3989783112809</v>
+        <v>3161.1982120447419</v>
       </c>
       <c r="F17" s="6">
         <f>SUM(FcstMonthlyFY2018!K18:M18)</f>
-        <v>2151.4500855523888</v>
+        <v>3765.0376497166817</v>
       </c>
       <c r="G17" s="6">
         <f>SUM(C17:F17)</f>
-        <v>6747.9764789036708</v>
+        <v>11808.958838081424</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -5651,23 +5654,23 @@
       </c>
       <c r="C18" s="6">
         <f>SUM(FcstMonthlyFY2018!B19:D19)</f>
-        <v>1209.768</v>
+        <v>1894.2420000000002</v>
       </c>
       <c r="D18" s="6">
         <f>SUM(FcstMonthlyFY2018!E19:G19)</f>
-        <v>1440.8530442880001</v>
+        <v>2256.0725298720004</v>
       </c>
       <c r="E18" s="6">
         <f>SUM(FcstMonthlyFY2018!H19:J19)</f>
-        <v>1716.079029395717</v>
+        <v>2687.0184802380309</v>
       </c>
       <c r="F18" s="6">
         <f>SUM(FcstMonthlyFY2018!K19:M19)</f>
-        <v>2043.8775812747699</v>
+        <v>3200.2820022591786</v>
       </c>
       <c r="G18" s="6">
         <f t="shared" ref="G18:G19" si="3">SUM(C18:F18)</f>
-        <v>6410.5776549584871</v>
+        <v>10037.61501236921</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -5679,23 +5682,23 @@
       </c>
       <c r="C19" s="6">
         <f>SUM(FcstMonthlyFY2018!B20:D20)</f>
-        <v>1146.096</v>
+        <v>1808.2847999999999</v>
       </c>
       <c r="D19" s="6">
         <f>SUM(FcstMonthlyFY2018!E20:G20)</f>
-        <v>1365.0186735360003</v>
+        <v>2153.6961293568002</v>
       </c>
       <c r="E19" s="6">
         <f>SUM(FcstMonthlyFY2018!H20:J20)</f>
-        <v>1625.759080480153</v>
+        <v>2565.0865492020189</v>
       </c>
       <c r="F19" s="6">
         <f>SUM(FcstMonthlyFY2018!K20:M20)</f>
-        <v>1936.3050769971503</v>
+        <v>3055.0591214843926</v>
       </c>
       <c r="G19" s="6">
         <f t="shared" si="3"/>
-        <v>6073.1788310133034</v>
+        <v>9582.1266000432115</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -5704,23 +5707,23 @@
       </c>
       <c r="C20" s="6">
         <f>SUM(C17:C19)</f>
-        <v>3629.3040000000001</v>
+        <v>5931.0468000000001</v>
       </c>
       <c r="D20" s="6">
         <f t="shared" ref="D20:F20" si="4">SUM(D17:D19)</f>
-        <v>4322.5591328640003</v>
+        <v>7063.9716355488017</v>
       </c>
       <c r="E20" s="6">
         <f t="shared" si="4"/>
-        <v>5148.2370881871511</v>
+        <v>8413.3032414847912</v>
       </c>
       <c r="F20" s="6">
         <f t="shared" si="4"/>
-        <v>6131.6327438243097</v>
+        <v>10020.378773460252</v>
       </c>
       <c r="G20" s="6">
         <f>SUM(G17:G19)</f>
-        <v>19231.73296487546</v>
+        <v>31428.700450493845</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5747,23 +5750,23 @@
       </c>
       <c r="C23" s="6">
         <f>C7</f>
-        <v>11779.32</v>
+        <v>11605.720000000001</v>
       </c>
       <c r="D23" s="6">
         <f>D7</f>
-        <v>14029.358589120002</v>
+        <v>13244.397978560002</v>
       </c>
       <c r="E23" s="6">
         <f>E7</f>
-        <v>16709.190549379353</v>
+        <v>15123.893275984305</v>
       </c>
       <c r="F23" s="6">
         <f>F7</f>
-        <v>19900.913291359604</v>
+        <v>17281.191122726617</v>
       </c>
       <c r="G23" s="6">
         <f>SUM(C23:F23)</f>
-        <v>62418.782429858962</v>
+        <v>57255.202377270929</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -5799,23 +5802,23 @@
       </c>
       <c r="C25" s="6">
         <f>C20</f>
-        <v>3629.3040000000001</v>
+        <v>5931.0468000000001</v>
       </c>
       <c r="D25" s="6">
         <f>D20</f>
-        <v>4322.5591328640003</v>
+        <v>7063.9716355488017</v>
       </c>
       <c r="E25" s="6">
         <f>E20</f>
-        <v>5148.2370881871511</v>
+        <v>8413.3032414847912</v>
       </c>
       <c r="F25" s="6">
         <f>F20</f>
-        <v>6131.6327438243097</v>
+        <v>10020.378773460252</v>
       </c>
       <c r="G25" s="6">
         <f t="shared" si="5"/>
-        <v>19231.73296487546</v>
+        <v>31428.700450493845</v>
       </c>
     </row>
   </sheetData>
@@ -5825,11 +5828,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="H2" sqref="H2:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5880,23 +5883,23 @@
       </c>
       <c r="C3" s="12">
         <f>SUM(FcstMonthlyFY2018!B4:D4)</f>
-        <v>3183.6000000000004</v>
+        <v>3121.6000000000004</v>
       </c>
       <c r="D3" s="12">
         <f>SUM(FcstMonthlyFY2018!E4:G4)</f>
-        <v>3791.7185376000007</v>
+        <v>3511.3754624000012</v>
       </c>
       <c r="E3" s="12">
         <f>SUM(FcstMonthlyFY2018!H4:J4)</f>
-        <v>4515.9974457782037</v>
+        <v>3949.8198481371151</v>
       </c>
       <c r="F3" s="12">
         <f>SUM(FcstMonthlyFY2018!K4:M4)</f>
-        <v>5378.6252138809732</v>
+        <v>4443.0101536549082</v>
       </c>
       <c r="G3" s="12">
         <f>SUM(C3:F3)</f>
-        <v>16869.941197259177</v>
+        <v>15025.805464192024</v>
       </c>
       <c r="H3" s="18" t="s">
         <v>30</v>
@@ -5911,23 +5914,23 @@
       </c>
       <c r="C4" s="12">
         <f>SUM(FcstMonthlyFY2018!B5:D5)</f>
-        <v>3501.96</v>
+        <v>3433.76</v>
       </c>
       <c r="D4" s="12">
         <f>SUM(FcstMonthlyFY2018!E5:G5)</f>
-        <v>4170.8903913600006</v>
+        <v>3862.5130086400004</v>
       </c>
       <c r="E4" s="12">
         <f>SUM(FcstMonthlyFY2018!H5:J5)</f>
-        <v>4967.597190356023</v>
+        <v>4344.8018329508259</v>
       </c>
       <c r="F4" s="12">
         <f>SUM(FcstMonthlyFY2018!K5:M5)</f>
-        <v>5916.4877352690692</v>
+        <v>4887.3111690203996</v>
       </c>
       <c r="G4" s="12">
         <f t="shared" ref="G4:G7" si="0">SUM(C4:F4)</f>
-        <v>18556.935316985095</v>
+        <v>16528.386010611226</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>30</v>
@@ -5942,23 +5945,23 @@
       </c>
       <c r="C5" s="12">
         <f>SUM(FcstMonthlyFY2018!B6:D6)</f>
-        <v>2228.52</v>
+        <v>2185.12</v>
       </c>
       <c r="D5" s="12">
         <f>SUM(FcstMonthlyFY2018!E6:G6)</f>
-        <v>2654.2029763200007</v>
+        <v>2457.9628236800004</v>
       </c>
       <c r="E5" s="12">
         <f>SUM(FcstMonthlyFY2018!H6:J6)</f>
-        <v>3161.1982120447419</v>
+        <v>2764.8738936959799</v>
       </c>
       <c r="F5" s="12">
         <f>SUM(FcstMonthlyFY2018!K6:M6)</f>
-        <v>3765.0376497166817</v>
+        <v>3110.107107558435</v>
       </c>
       <c r="G5" s="12">
         <f t="shared" si="0"/>
-        <v>11808.958838081424</v>
+        <v>10518.063824934416</v>
       </c>
       <c r="H5" s="18" t="s">
         <v>30</v>
@@ -6004,23 +6007,23 @@
       </c>
       <c r="C7" s="12">
         <f>SUM(FcstMonthlyFY2018!B8:D8)</f>
-        <v>11779.32</v>
+        <v>11605.720000000001</v>
       </c>
       <c r="D7" s="12">
         <f>SUM(FcstMonthlyFY2018!E8:G8)</f>
-        <v>14029.358589120002</v>
+        <v>13244.397978560002</v>
       </c>
       <c r="E7" s="12">
         <f>SUM(FcstMonthlyFY2018!H8:J8)</f>
-        <v>16709.190549379353</v>
+        <v>15123.893275984305</v>
       </c>
       <c r="F7" s="12">
         <f>SUM(FcstMonthlyFY2018!K8:M8)</f>
-        <v>19900.913291359604</v>
+        <v>17281.191122726617</v>
       </c>
       <c r="G7" s="12">
         <f t="shared" si="0"/>
-        <v>62418.782429858962</v>
+        <v>57255.202377270929</v>
       </c>
       <c r="H7" s="18" t="s">
         <v>30</v>
@@ -6033,11 +6036,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6045,9 +6048,10 @@
     <col min="1" max="1" width="12.140625" style="10" customWidth="1"/>
     <col min="2" max="2" width="39.5703125" customWidth="1"/>
     <col min="3" max="7" width="14" style="12" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>23</v>
       </c>
@@ -6055,7 +6059,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
@@ -6074,10 +6078,13 @@
       <c r="G2" s="14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -6102,10 +6109,13 @@
         <f>SUM(C3:F3)</f>
         <v>8434.9705986295885</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -6130,10 +6140,13 @@
         <f t="shared" ref="G4:G5" si="0">SUM(C4:F4)</f>
         <v>10121.964718355506</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -6158,10 +6171,13 @@
         <f t="shared" si="0"/>
         <v>11808.958838081424</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -6186,8 +6202,14 @@
         <f>SUM(C6:F6)</f>
         <v>10459.363542300691</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>10</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
@@ -6210,6 +6232,9 @@
       <c r="G7" s="12">
         <f t="shared" ref="G7" si="1">SUM(C7:F7)</f>
         <v>40825.257697367211</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -6218,11 +6243,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6230,9 +6255,10 @@
     <col min="1" max="1" width="12.140625" style="10" customWidth="1"/>
     <col min="2" max="2" width="39.5703125" customWidth="1"/>
     <col min="3" max="7" width="14" style="12" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>23</v>
       </c>
@@ -6240,7 +6266,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
@@ -6259,115 +6285,136 @@
       <c r="G2" s="14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="12">
         <f>SUM(FcstMonthlyFY2018!B18:D18)</f>
-        <v>1273.44</v>
+        <v>2228.52</v>
       </c>
       <c r="D3" s="12">
         <f>SUM(FcstMonthlyFY2018!E18:G18)</f>
-        <v>1516.6874150400001</v>
+        <v>2654.2029763200007</v>
       </c>
       <c r="E3" s="12">
         <f>SUM(FcstMonthlyFY2018!H18:J18)</f>
-        <v>1806.3989783112809</v>
+        <v>3161.1982120447419</v>
       </c>
       <c r="F3" s="12">
         <f>SUM(FcstMonthlyFY2018!K18:M18)</f>
-        <v>2151.4500855523888</v>
+        <v>3765.0376497166817</v>
       </c>
       <c r="G3" s="12">
         <f>SUM(C3:F3)</f>
-        <v>6747.9764789036708</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11808.958838081424</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="12">
         <f>SUM(FcstMonthlyFY2018!B19:D19)</f>
-        <v>1209.768</v>
+        <v>1894.2420000000002</v>
       </c>
       <c r="D4" s="12">
         <f>SUM(FcstMonthlyFY2018!E19:G19)</f>
-        <v>1440.8530442880001</v>
+        <v>2256.0725298720004</v>
       </c>
       <c r="E4" s="12">
         <f>SUM(FcstMonthlyFY2018!H19:J19)</f>
-        <v>1716.079029395717</v>
+        <v>2687.0184802380309</v>
       </c>
       <c r="F4" s="12">
         <f>SUM(FcstMonthlyFY2018!K19:M19)</f>
-        <v>2043.8775812747699</v>
+        <v>3200.2820022591786</v>
       </c>
       <c r="G4" s="12">
         <f t="shared" ref="G4:G5" si="0">SUM(C4:F4)</f>
-        <v>6410.5776549584871</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10037.61501236921</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="12">
         <f>SUM(FcstMonthlyFY2018!B20:D20)</f>
-        <v>1146.096</v>
+        <v>1808.2847999999999</v>
       </c>
       <c r="D5" s="12">
         <f>SUM(FcstMonthlyFY2018!E20:G20)</f>
-        <v>1365.0186735360003</v>
+        <v>2153.6961293568002</v>
       </c>
       <c r="E5" s="12">
         <f>SUM(FcstMonthlyFY2018!H20:J20)</f>
-        <v>1625.759080480153</v>
+        <v>2565.0865492020189</v>
       </c>
       <c r="F5" s="12">
         <f>SUM(FcstMonthlyFY2018!K20:M20)</f>
-        <v>1936.3050769971503</v>
+        <v>3055.0591214843926</v>
       </c>
       <c r="G5" s="12">
         <f t="shared" si="0"/>
-        <v>6073.1788310133034</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9582.1266000432115</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>14</v>
+      </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="12">
         <f>SUM(C3:C5)</f>
-        <v>3629.3040000000001</v>
+        <v>5931.0468000000001</v>
       </c>
       <c r="D6" s="12">
         <f t="shared" ref="D6:F6" si="1">SUM(D3:D5)</f>
-        <v>4322.5591328640003</v>
+        <v>7063.9716355488017</v>
       </c>
       <c r="E6" s="12">
         <f t="shared" si="1"/>
-        <v>5148.2370881871511</v>
+        <v>8413.3032414847912</v>
       </c>
       <c r="F6" s="12">
         <f t="shared" si="1"/>
-        <v>6131.6327438243097</v>
+        <v>10020.378773460252</v>
       </c>
       <c r="G6" s="12">
         <f>SUM(G3:G5)</f>
-        <v>19231.73296487546</v>
-      </c>
+        <v>31428.700450493845</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>